<commit_message>
add BBG consensus data, temporal multi-snapshot, combined chart
- Add Bloomberg consensus forecast data (bbg-consensus-forecast.xlsx)
- Add plot_bbg_consensus_histogram() for BBG forecaster counts
- Add plot_kalshi_chifed_bbg() combining Kalshi/ChiFed lines with BBG bars
- Refactor plot_temporal_comparison() to support 3+ snapshots
- Remove stats box from temporal chart
- Add load_from_strike_csv() for long-format Kalshi data
- Change Chicago Fed default release from "advance" to "final"
- Update README with new figures and data sources

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/raw/chi-labor-market-indicators.xlsx
+++ b/data/raw/chi-labor-market-indicators.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66988E7B-F1D8-4D20-8918-03E0BD1A00D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F780230E-6AE3-401A-82A4-F2980853B636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="5" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="138">
   <si>
     <t>Key</t>
   </si>
@@ -607,52 +607,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -675,14 +629,23 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -734,6 +697,43 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -758,71 +758,71 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,7 +1105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -1691,13 +1691,13 @@
         <v>39641</v>
       </c>
       <c r="B2">
-        <v>2.4067244091119502</v>
+        <v>2.40630274998701</v>
       </c>
       <c r="C2">
-        <v>35.374754998905402</v>
+        <v>35.384313617006399</v>
       </c>
       <c r="D2">
-        <v>6.3701169113066403</v>
+        <v>6.3674609766055399</v>
       </c>
       <c r="E2">
         <v>2.7800352340979702</v>
@@ -1711,13 +1711,13 @@
         <v>39676</v>
       </c>
       <c r="B3">
-        <v>2.4479826261283799</v>
+        <v>2.4474239620898701</v>
       </c>
       <c r="C3">
-        <v>34.458500841128597</v>
+        <v>34.465948569442801</v>
       </c>
       <c r="D3">
-        <v>6.6329338266546296</v>
+        <v>6.6301824900967699</v>
       </c>
       <c r="E3">
         <v>3.23000889314353</v>
@@ -1731,13 +1731,13 @@
         <v>39704</v>
       </c>
       <c r="B4">
-        <v>2.4859873688996199</v>
+        <v>2.4852473876658201</v>
       </c>
       <c r="C4">
-        <v>33.319133292333802</v>
+        <v>33.327716069181903</v>
       </c>
       <c r="D4">
-        <v>6.9431056870902301</v>
+        <v>6.93951895564404</v>
       </c>
       <c r="E4">
         <v>2.7929791294266799</v>
@@ -1751,13 +1751,13 @@
         <v>39739</v>
       </c>
       <c r="B5">
-        <v>2.53724333901889</v>
+        <v>2.5361973261608299</v>
       </c>
       <c r="C5">
-        <v>31.8948823801293</v>
+        <v>31.898718719725</v>
       </c>
       <c r="D5">
-        <v>7.3688257289554704</v>
+        <v>7.3651909671603502</v>
       </c>
       <c r="E5">
         <v>3.05803906803609</v>
@@ -1771,13 +1771,13 @@
         <v>39767</v>
       </c>
       <c r="B6">
-        <v>2.6104318784147802</v>
+        <v>2.6091680810020699</v>
       </c>
       <c r="C6">
-        <v>30.625359291013702</v>
+        <v>30.634282463689502</v>
       </c>
       <c r="D6">
-        <v>7.8542793373186202</v>
+        <v>7.8486680481449396</v>
       </c>
       <c r="E6">
         <v>3.2801612051511202</v>
@@ -1791,13 +1791,13 @@
         <v>39795</v>
       </c>
       <c r="B7">
-        <v>2.6722306211631399</v>
+        <v>2.6705349645985499</v>
       </c>
       <c r="C7">
-        <v>28.7978821802322</v>
+        <v>28.8039301219892</v>
       </c>
       <c r="D7">
-        <v>8.4913283852120394</v>
+        <v>8.4847668014429498</v>
       </c>
       <c r="E7">
         <v>3.0970338191158602</v>
@@ -1811,13 +1811,13 @@
         <v>39830</v>
       </c>
       <c r="B8">
-        <v>2.72012047740039</v>
+        <v>2.7183166199255999</v>
       </c>
       <c r="C8">
-        <v>28.338321906540301</v>
+        <v>28.3462984163526</v>
       </c>
       <c r="D8">
-        <v>8.75807113497385</v>
+        <v>8.7505240826292692</v>
       </c>
       <c r="E8">
         <v>3.4153900734587399</v>
@@ -1831,13 +1831,13 @@
         <v>39858</v>
       </c>
       <c r="B9">
-        <v>2.7971895130744802</v>
+        <v>2.7949393526756099</v>
       </c>
       <c r="C9">
-        <v>26.3685355079317</v>
+        <v>26.376411143680102</v>
       </c>
       <c r="D9">
-        <v>9.5906736796696794</v>
+        <v>9.5811105935077308</v>
       </c>
       <c r="E9">
         <v>3.2530153609995298</v>
@@ -1851,13 +1851,13 @@
         <v>39886</v>
       </c>
       <c r="B10">
-        <v>2.8481340258481902</v>
+        <v>2.84558320715528</v>
       </c>
       <c r="C10">
-        <v>25.374760766806698</v>
+        <v>25.381103449216901</v>
       </c>
       <c r="D10">
-        <v>10.0915729827595</v>
+        <v>10.0811804155302</v>
       </c>
       <c r="E10">
         <v>3.3455934169004999</v>
@@ -1871,13 +1871,13 @@
         <v>39921</v>
       </c>
       <c r="B11">
-        <v>2.86622813750841</v>
+        <v>2.86365614933769</v>
       </c>
       <c r="C11">
-        <v>25.034877200357201</v>
+        <v>25.0420488094219</v>
       </c>
       <c r="D11">
-        <v>10.2728121441789</v>
+        <v>10.261902193726099</v>
       </c>
       <c r="E11">
         <v>3.1571785351665</v>
@@ -1891,13 +1891,13 @@
         <v>39949</v>
       </c>
       <c r="B12">
-        <v>2.8680961970835899</v>
+        <v>2.8655877257284699</v>
       </c>
       <c r="C12">
-        <v>25.090763288872001</v>
+        <v>25.1001858235628</v>
       </c>
       <c r="D12">
-        <v>10.2582732265038</v>
+        <v>10.246767251682501</v>
       </c>
       <c r="E12">
         <v>3.0223178661676999</v>
@@ -1911,13 +1911,13 @@
         <v>39977</v>
       </c>
       <c r="B13">
-        <v>2.86359812135627</v>
+        <v>2.8610550968061799</v>
       </c>
       <c r="C13">
-        <v>25.039867949017999</v>
+        <v>25.043876899069598</v>
       </c>
       <c r="D13">
-        <v>10.2625176174676</v>
+        <v>10.2528653258465</v>
       </c>
       <c r="E13">
         <v>2.9403976095063902</v>
@@ -1931,13 +1931,13 @@
         <v>40012</v>
       </c>
       <c r="B14">
-        <v>2.8548125614009501</v>
+        <v>2.8520337656157499</v>
       </c>
       <c r="C14">
-        <v>24.672014592229701</v>
+        <v>24.672524479568501</v>
       </c>
       <c r="D14">
-        <v>10.371019316784601</v>
+        <v>10.361778525963199</v>
       </c>
       <c r="E14">
         <v>3.0152984194464199</v>
@@ -1951,13 +1951,13 @@
         <v>40040</v>
       </c>
       <c r="B15">
-        <v>2.82507449825812</v>
+        <v>2.8226497176538698</v>
       </c>
       <c r="C15">
-        <v>25.505309625133499</v>
+        <v>25.508592707781499</v>
       </c>
       <c r="D15">
-        <v>9.9718891418967299</v>
+        <v>9.9630283602378604</v>
       </c>
       <c r="E15">
         <v>2.7689692757697602</v>
@@ -1971,13 +1971,13 @@
         <v>40068</v>
       </c>
       <c r="B16">
-        <v>2.83491991352976</v>
+        <v>2.8322489795518799</v>
       </c>
       <c r="C16">
-        <v>25.0236131431781</v>
+        <v>25.0222965357164</v>
       </c>
       <c r="D16">
-        <v>10.176127751447201</v>
+        <v>10.1679956616036</v>
       </c>
       <c r="E16">
         <v>2.69097173095735</v>
@@ -1991,13 +1991,13 @@
         <v>40103</v>
       </c>
       <c r="B17">
-        <v>2.8393669240330199</v>
+        <v>2.8365487475353</v>
       </c>
       <c r="C17">
-        <v>24.821434410499499</v>
+        <v>24.819674726611499</v>
       </c>
       <c r="D17">
-        <v>10.2649481831471</v>
+        <v>10.2564572859593</v>
       </c>
       <c r="E17">
         <v>3.06105413812945</v>
@@ -2011,13 +2011,13 @@
         <v>40131</v>
       </c>
       <c r="B18">
-        <v>2.8214023370103898</v>
+        <v>2.81859411367821</v>
       </c>
       <c r="C18">
-        <v>24.957052031985899</v>
+        <v>24.952556181756201</v>
       </c>
       <c r="D18">
-        <v>10.1568010211518</v>
+        <v>10.1493603386734</v>
       </c>
       <c r="E18">
         <v>2.6582410704530099</v>
@@ -2031,13 +2031,13 @@
         <v>40159</v>
       </c>
       <c r="B19">
-        <v>2.79044353777654</v>
+        <v>2.78777992782656</v>
       </c>
       <c r="C19">
-        <v>25.487651224417899</v>
+        <v>25.4810476392704</v>
       </c>
       <c r="D19">
-        <v>9.8678626026359293</v>
+        <v>9.8616750949775795</v>
       </c>
       <c r="E19">
         <v>2.79393005620588</v>
@@ -2051,13 +2051,13 @@
         <v>40194</v>
       </c>
       <c r="B20">
-        <v>2.77583092283772</v>
+        <v>2.77332036168107</v>
       </c>
       <c r="C20">
-        <v>26.001538438766001</v>
+        <v>25.998065297009301</v>
       </c>
       <c r="D20">
-        <v>9.6458814145165803</v>
+        <v>9.6391616120977197</v>
       </c>
       <c r="E20">
         <v>2.7551809544839498</v>
@@ -2071,13 +2071,13 @@
         <v>40222</v>
       </c>
       <c r="B21">
-        <v>2.7547372325045498</v>
+        <v>2.75227536906766</v>
       </c>
       <c r="C21">
-        <v>26.091616753407699</v>
+        <v>26.0840985873009</v>
       </c>
       <c r="D21">
-        <v>9.5496894819008507</v>
+        <v>9.5444571957349709</v>
       </c>
       <c r="E21">
         <v>2.6269975068560201</v>
@@ -2091,13 +2091,13 @@
         <v>40250</v>
       </c>
       <c r="B22">
-        <v>2.7432242920163699</v>
+        <v>2.74076485326631</v>
       </c>
       <c r="C22">
-        <v>26.3543361265992</v>
+        <v>26.345701086970799</v>
       </c>
       <c r="D22">
-        <v>9.4276779652680194</v>
+        <v>9.4228183612875398</v>
       </c>
       <c r="E22">
         <v>2.5762994879490901</v>
@@ -2111,13 +2111,13 @@
         <v>40285</v>
       </c>
       <c r="B23">
-        <v>2.7399105060396098</v>
+        <v>2.73769713111114</v>
       </c>
       <c r="C23">
-        <v>26.972127711380399</v>
+        <v>26.968284355382199</v>
       </c>
       <c r="D23">
-        <v>9.2215501541500107</v>
+        <v>9.2159793890530608</v>
       </c>
       <c r="E23">
         <v>2.48886318953305</v>
@@ -2131,13 +2131,13 @@
         <v>40313</v>
       </c>
       <c r="B24">
-        <v>2.7232092877399201</v>
+        <v>2.7210537760254798</v>
       </c>
       <c r="C24">
-        <v>27.037879262920299</v>
+        <v>27.029873579548202</v>
       </c>
       <c r="D24">
-        <v>9.1502341492126202</v>
+        <v>9.1461141479870598</v>
       </c>
       <c r="E24">
         <v>2.67970675055569</v>
@@ -2151,13 +2151,13 @@
         <v>40341</v>
       </c>
       <c r="B25">
-        <v>2.7157408074394298</v>
+        <v>2.7136892397772301</v>
       </c>
       <c r="C25">
-        <v>27.3535395726682</v>
+        <v>27.3461342688089</v>
       </c>
       <c r="D25">
-        <v>9.0316122404978891</v>
+        <v>9.0276286519184108</v>
       </c>
       <c r="E25">
         <v>2.5809344541940602</v>
@@ -2171,13 +2171,13 @@
         <v>40376</v>
       </c>
       <c r="B26">
-        <v>2.7629707935665202</v>
+        <v>2.7606691408467898</v>
       </c>
       <c r="C26">
-        <v>27.1206876546897</v>
+        <v>27.1190673656961</v>
       </c>
       <c r="D26">
-        <v>9.2457581736540995</v>
+        <v>9.2392686938262596</v>
       </c>
       <c r="E26">
         <v>2.6401779196904398</v>
@@ -2191,13 +2191,13 @@
         <v>40404</v>
       </c>
       <c r="B27">
-        <v>2.7453799290171901</v>
+        <v>2.7429843522586901</v>
       </c>
       <c r="C27">
-        <v>26.322792318225801</v>
+        <v>26.3209005129636</v>
       </c>
       <c r="D27">
-        <v>9.44462522674635</v>
+        <v>9.4377760061282494</v>
       </c>
       <c r="E27">
         <v>2.4607348523616701</v>
@@ -2211,13 +2211,13 @@
         <v>40439</v>
       </c>
       <c r="B28">
-        <v>2.7242449948611598</v>
+        <v>2.7218776965823399</v>
       </c>
       <c r="C28">
-        <v>26.562617819534601</v>
+        <v>26.554036916022699</v>
       </c>
       <c r="D28">
-        <v>9.30193517867019</v>
+        <v>9.2973276244302294</v>
       </c>
       <c r="E28">
         <v>2.6695206369643398</v>
@@ -2231,13 +2231,13 @@
         <v>40467</v>
       </c>
       <c r="B29">
-        <v>2.7123515606915301</v>
+        <v>2.7100050338457899</v>
       </c>
       <c r="C29">
-        <v>26.609665090123301</v>
+        <v>26.600800049931401</v>
       </c>
       <c r="D29">
-        <v>9.2502217463141605</v>
+        <v>9.2457543424684498</v>
       </c>
       <c r="E29">
         <v>2.5141031063378598</v>
@@ -2251,13 +2251,13 @@
         <v>40495</v>
       </c>
       <c r="B30">
-        <v>2.6991024030336699</v>
+        <v>2.6967745367439102</v>
       </c>
       <c r="C30">
-        <v>26.783845092248001</v>
+        <v>26.771900556660899</v>
       </c>
       <c r="D30">
-        <v>9.1547916078120206</v>
+        <v>9.1513260375504792</v>
       </c>
       <c r="E30">
         <v>2.6659842648673799</v>
@@ -2271,13 +2271,13 @@
         <v>40523</v>
       </c>
       <c r="B31">
-        <v>2.7069187605526399</v>
+        <v>2.7045860354975799</v>
       </c>
       <c r="C31">
-        <v>27.2294245907975</v>
+        <v>27.219318108758401</v>
       </c>
       <c r="D31">
-        <v>9.0422491778059904</v>
+        <v>9.0382124687320893</v>
       </c>
       <c r="E31">
         <v>2.6244739316357899</v>
@@ -2291,13 +2291,13 @@
         <v>40558</v>
       </c>
       <c r="B32">
-        <v>2.6860745970979698</v>
+        <v>2.68386957874253</v>
       </c>
       <c r="C32">
-        <v>27.317003607064201</v>
+        <v>27.307773411973699</v>
       </c>
       <c r="D32">
-        <v>8.9526633861366403</v>
+        <v>8.9487247483350902</v>
       </c>
       <c r="E32">
         <v>2.5844489972709401</v>
@@ -2311,13 +2311,13 @@
         <v>40586</v>
       </c>
       <c r="B33">
-        <v>2.6614837463085901</v>
+        <v>2.6594388060010901</v>
       </c>
       <c r="C33">
-        <v>27.858905286670598</v>
+        <v>27.851203339893701</v>
       </c>
       <c r="D33">
-        <v>8.7203467276668398</v>
+        <v>8.7164301337358499</v>
       </c>
       <c r="E33">
         <v>2.3220904777338398</v>
@@ -2331,13 +2331,13 @@
         <v>40614</v>
       </c>
       <c r="B34">
-        <v>2.63089504743045</v>
+        <v>2.6289076843937602</v>
       </c>
       <c r="C34">
-        <v>28.282565389077899</v>
+        <v>28.270804192783299</v>
       </c>
       <c r="D34">
-        <v>8.5105161644194194</v>
+        <v>8.5078711893605306</v>
       </c>
       <c r="E34">
         <v>2.3680480700764899</v>
@@ -2351,13 +2351,13 @@
         <v>40649</v>
       </c>
       <c r="B35">
-        <v>2.62345937129236</v>
+        <v>2.6216688728906101</v>
       </c>
       <c r="C35">
-        <v>28.858542529945598</v>
+        <v>28.851411183391299</v>
       </c>
       <c r="D35">
-        <v>8.3332037763113007</v>
+        <v>8.32987705112558</v>
       </c>
       <c r="E35">
         <v>2.6034383372416299</v>
@@ -2371,13 +2371,13 @@
         <v>40677</v>
       </c>
       <c r="B36">
-        <v>2.6351385831367802</v>
+        <v>2.6331984440676002</v>
       </c>
       <c r="C36">
-        <v>28.294868919106399</v>
+        <v>28.2863056372058</v>
       </c>
       <c r="D36">
-        <v>8.5196829743596698</v>
+        <v>8.51630232213979</v>
       </c>
       <c r="E36">
         <v>2.5218085146025699</v>
@@ -2391,13 +2391,13 @@
         <v>40712</v>
       </c>
       <c r="B37">
-        <v>2.64245518185888</v>
+        <v>2.6404820956247201</v>
       </c>
       <c r="C37">
-        <v>28.154457521654699</v>
+        <v>28.146214730142901</v>
       </c>
       <c r="D37">
-        <v>8.5802599997544693</v>
+        <v>8.5766982751287308</v>
       </c>
       <c r="E37">
         <v>2.7938210615761201</v>
@@ -2411,13 +2411,13 @@
         <v>40740</v>
       </c>
       <c r="B38">
-        <v>2.6591611646258202</v>
+        <v>2.6570877948251899</v>
       </c>
       <c r="C38">
-        <v>27.916207340419501</v>
+        <v>27.9092742178793</v>
       </c>
       <c r="D38">
-        <v>8.6970698789354799</v>
+        <v>8.6928493280319401</v>
       </c>
       <c r="E38">
         <v>2.4960370704375099</v>
@@ -2431,13 +2431,13 @@
         <v>40768</v>
       </c>
       <c r="B39">
-        <v>2.6548592428789202</v>
+        <v>2.6527258094989699</v>
       </c>
       <c r="C39">
-        <v>27.475505216287701</v>
+        <v>27.466162576652401</v>
       </c>
       <c r="D39">
-        <v>8.8112417175598701</v>
+        <v>8.8075156542586406</v>
       </c>
       <c r="E39">
         <v>2.4530300457199399</v>
@@ -2451,13 +2451,13 @@
         <v>40803</v>
       </c>
       <c r="B40">
-        <v>2.6623201937105501</v>
+        <v>2.66014604004905</v>
       </c>
       <c r="C40">
-        <v>27.494731342474601</v>
+        <v>27.484669878409601</v>
       </c>
       <c r="D40">
-        <v>8.8281846470171796</v>
+        <v>8.8245555960424795</v>
       </c>
       <c r="E40">
         <v>2.55482629853124</v>
@@ -2471,13 +2471,13 @@
         <v>40831</v>
       </c>
       <c r="B41">
-        <v>2.64317800919435</v>
+        <v>2.6409907015200198</v>
       </c>
       <c r="C41">
-        <v>27.722030763017901</v>
+        <v>27.710022870133699</v>
       </c>
       <c r="D41">
-        <v>8.7046264987750508</v>
+        <v>8.7014909577404396</v>
       </c>
       <c r="E41">
         <v>2.5450333327351</v>
@@ -2491,13 +2491,13 @@
         <v>40859</v>
       </c>
       <c r="B42">
-        <v>2.6174220569169</v>
+        <v>2.6155351523421402</v>
       </c>
       <c r="C42">
-        <v>28.7611963376396</v>
+        <v>28.751938862284199</v>
       </c>
       <c r="D42">
-        <v>8.3414190644255992</v>
+        <v>8.3383671605897902</v>
       </c>
       <c r="E42">
         <v>2.4001448471716502</v>
@@ -2511,13 +2511,13 @@
         <v>40887</v>
       </c>
       <c r="B43">
-        <v>2.5883427857890702</v>
+        <v>2.5865867538867802</v>
       </c>
       <c r="C43">
-        <v>29.533277520297698</v>
+        <v>29.523793242378598</v>
       </c>
       <c r="D43">
-        <v>8.0579458978867091</v>
+        <v>8.0552978637674695</v>
       </c>
       <c r="E43">
         <v>2.5444486384976801</v>
@@ -2531,13 +2531,13 @@
         <v>40922</v>
       </c>
       <c r="B44">
-        <v>2.5864611702451801</v>
+        <v>2.5847412311264502</v>
       </c>
       <c r="C44">
-        <v>29.4506357302933</v>
+        <v>29.442233003376099</v>
       </c>
       <c r="D44">
-        <v>8.0733319197898492</v>
+        <v>8.0705133497809793</v>
       </c>
       <c r="E44">
         <v>2.3027087777579198</v>
@@ -2551,13 +2551,13 @@
         <v>40957</v>
       </c>
       <c r="B45">
-        <v>2.5469140497164902</v>
+        <v>2.5454668103794198</v>
       </c>
       <c r="C45">
-        <v>30.6711846711265</v>
+        <v>30.661857420317499</v>
       </c>
       <c r="D45">
-        <v>7.6672481201291802</v>
+        <v>7.6653776519168799</v>
       </c>
       <c r="E45">
         <v>2.4186532553757498</v>
@@ -2571,13 +2571,13 @@
         <v>40985</v>
       </c>
       <c r="B46">
-        <v>2.55354694875302</v>
+        <v>2.55201627125596</v>
       </c>
       <c r="C46">
-        <v>30.571278769517399</v>
+        <v>30.562829366861099</v>
       </c>
       <c r="D46">
-        <v>7.7088615362724298</v>
+        <v>7.7065624860362902</v>
       </c>
       <c r="E46">
         <v>2.5467057762563701</v>
@@ -2591,13 +2591,13 @@
         <v>41013</v>
       </c>
       <c r="B47">
-        <v>2.5407608040165002</v>
+        <v>2.5394497075226701</v>
       </c>
       <c r="C47">
-        <v>30.8440687297301</v>
+        <v>30.8370004794698</v>
       </c>
       <c r="D47">
-        <v>7.6105250184015496</v>
+        <v>7.6085074754665003</v>
       </c>
       <c r="E47">
         <v>2.4707529605966001</v>
@@ -2611,13 +2611,13 @@
         <v>41041</v>
       </c>
       <c r="B48">
-        <v>2.54824968106719</v>
+        <v>2.5467116884792298</v>
       </c>
       <c r="C48">
-        <v>30.2899720682449</v>
+        <v>30.281923186236199</v>
       </c>
       <c r="D48">
-        <v>7.7600111861129504</v>
+        <v>7.7575924134472602</v>
       </c>
       <c r="E48">
         <v>2.3518201988946998</v>
@@ -2631,13 +2631,13 @@
         <v>41076</v>
       </c>
       <c r="B49">
-        <v>2.5618021926370802</v>
+        <v>2.56021544761902</v>
       </c>
       <c r="C49">
-        <v>30.177523503483702</v>
+        <v>30.171422798763199</v>
       </c>
       <c r="D49">
-        <v>7.8248471468690903</v>
+        <v>7.8218371727910601</v>
       </c>
       <c r="E49">
         <v>2.5629485671503498</v>
@@ -2651,13 +2651,13 @@
         <v>41104</v>
       </c>
       <c r="B50">
-        <v>2.55928580091132</v>
+        <v>2.5577814166139001</v>
       </c>
       <c r="C50">
-        <v>30.155013766376801</v>
+        <v>30.148746341619798</v>
       </c>
       <c r="D50">
-        <v>7.8231410568558104</v>
+        <v>7.8204003663152299</v>
       </c>
       <c r="E50">
         <v>2.49803530448622</v>
@@ -2671,13 +2671,13 @@
         <v>41139</v>
       </c>
       <c r="B51">
-        <v>2.55202319346188</v>
+        <v>2.5504609158944498</v>
       </c>
       <c r="C51">
-        <v>30.252510917194002</v>
+        <v>30.241951855761901</v>
       </c>
       <c r="D51">
-        <v>7.7794831191731797</v>
+        <v>7.7775945724216502</v>
       </c>
       <c r="E51">
         <v>2.6555043715011299</v>
@@ -2691,13 +2691,13 @@
         <v>41167</v>
       </c>
       <c r="B52">
-        <v>2.55583094395078</v>
+        <v>2.5542907450513299</v>
       </c>
       <c r="C52">
-        <v>30.1659207747932</v>
+        <v>30.158483115996901</v>
       </c>
       <c r="D52">
-        <v>7.8108011023343904</v>
+        <v>7.8082364885992499</v>
       </c>
       <c r="E52">
         <v>2.3744074844670902</v>
@@ -2711,13 +2711,13 @@
         <v>41195</v>
       </c>
       <c r="B53">
-        <v>2.5319047128912402</v>
+        <v>2.5305718118912499</v>
       </c>
       <c r="C53">
-        <v>31.164267357187899</v>
+        <v>31.1562927919285</v>
       </c>
       <c r="D53">
-        <v>7.5139238594388198</v>
+        <v>7.5120431706912401</v>
       </c>
       <c r="E53">
         <v>2.43638690101514</v>
@@ -2731,13 +2731,13 @@
         <v>41223</v>
       </c>
       <c r="B54">
-        <v>2.5665637146072302</v>
+        <v>2.5652682321135498</v>
       </c>
       <c r="C54">
-        <v>31.0191343902173</v>
+        <v>31.0168471675108</v>
       </c>
       <c r="D54">
-        <v>7.64183524367043</v>
+        <v>7.6387928562184797</v>
       </c>
       <c r="E54">
         <v>2.4672249786845</v>
@@ -2751,13 +2751,13 @@
         <v>41251</v>
       </c>
       <c r="B55">
-        <v>2.49495653881909</v>
+        <v>2.4937268457494</v>
       </c>
       <c r="C55">
-        <v>32.121307566357203</v>
+        <v>32.114112678980398</v>
       </c>
       <c r="D55">
-        <v>7.2074690996074402</v>
+        <v>7.2056703914367501</v>
       </c>
       <c r="E55">
         <v>2.53783817587692</v>
@@ -2771,13 +2771,13 @@
         <v>41286</v>
       </c>
       <c r="B56">
-        <v>2.4915203663060201</v>
+        <v>2.49034623677109</v>
       </c>
       <c r="C56">
-        <v>31.9459207923686</v>
+        <v>31.937772741788699</v>
       </c>
       <c r="D56">
-        <v>7.2349172368122501</v>
+        <v>7.2334658722480896</v>
       </c>
       <c r="E56">
         <v>2.57894444373086</v>
@@ -2791,13 +2791,13 @@
         <v>41321</v>
       </c>
       <c r="B57">
-        <v>2.4843746350421201</v>
+        <v>2.4832146601331799</v>
       </c>
       <c r="C57">
-        <v>32.050443527189699</v>
+        <v>32.039002671902402</v>
       </c>
       <c r="D57">
-        <v>7.1938257308072302</v>
+        <v>7.1930914409394902</v>
       </c>
       <c r="E57">
         <v>2.6246262603583101</v>
@@ -2811,13 +2811,13 @@
         <v>41349</v>
       </c>
       <c r="B58">
-        <v>2.4634126074071601</v>
+        <v>2.4623146683257602</v>
       </c>
       <c r="C58">
-        <v>32.605011587541703</v>
+        <v>32.592434239983099</v>
       </c>
       <c r="D58">
-        <v>7.0245888258702402</v>
+        <v>7.0241971345061396</v>
       </c>
       <c r="E58">
         <v>2.3248597122069299</v>
@@ -2831,13 +2831,13 @@
         <v>41377</v>
       </c>
       <c r="B59">
-        <v>2.47877059669496</v>
+        <v>2.47765110389216</v>
       </c>
       <c r="C59">
-        <v>31.990094465369001</v>
+        <v>31.9828383687639</v>
       </c>
       <c r="D59">
-        <v>7.1913322130906696</v>
+        <v>7.1898314324819603</v>
       </c>
       <c r="E59">
         <v>2.2797348990608701</v>
@@ -2851,13 +2851,13 @@
         <v>41412</v>
       </c>
       <c r="B60">
-        <v>2.4633922175528999</v>
+        <v>2.4623310050938301</v>
       </c>
       <c r="C60">
-        <v>32.527113898575699</v>
+        <v>32.518758122477699</v>
       </c>
       <c r="D60">
-        <v>7.0401731526181601</v>
+        <v>7.0390347084792699</v>
       </c>
       <c r="E60">
         <v>2.5119176271944901</v>
@@ -2871,13 +2871,13 @@
         <v>41440</v>
       </c>
       <c r="B61">
-        <v>2.4640260277939299</v>
+        <v>2.4629759896632302</v>
       </c>
       <c r="C61">
-        <v>32.546394722907898</v>
+        <v>32.538336675065104</v>
       </c>
       <c r="D61">
-        <v>7.0379789073073002</v>
+        <v>7.0368103426738804</v>
       </c>
       <c r="E61">
         <v>2.4875907182693102</v>
@@ -2891,13 +2891,13 @@
         <v>41468</v>
       </c>
       <c r="B62">
-        <v>2.4621616763550702</v>
+        <v>2.46115236300427</v>
       </c>
       <c r="C62">
-        <v>32.721077361626001</v>
+        <v>32.714274295675402</v>
       </c>
       <c r="D62">
-        <v>6.9981097354257704</v>
+        <v>6.9967946284937899</v>
       </c>
       <c r="E62">
         <v>2.3636974797576</v>
@@ -2911,13 +2911,13 @@
         <v>41503</v>
       </c>
       <c r="B63">
-        <v>2.4595092279847401</v>
+        <v>2.45847134335013</v>
       </c>
       <c r="C63">
-        <v>32.8913965558041</v>
+        <v>32.883801109176098</v>
       </c>
       <c r="D63">
-        <v>6.9574150179558396</v>
+        <v>6.9561778933499303</v>
       </c>
       <c r="E63">
         <v>2.3012644668511499</v>
@@ -2931,13 +2931,13 @@
         <v>41531</v>
       </c>
       <c r="B64">
-        <v>2.4353515730445698</v>
+        <v>2.4343647243855799</v>
       </c>
       <c r="C64">
-        <v>33.308647827997902</v>
+        <v>33.299611311484</v>
       </c>
       <c r="D64">
-        <v>6.8133158400107297</v>
+        <v>6.8124653185583801</v>
       </c>
       <c r="E64">
         <v>2.43237770034498</v>
@@ -2951,13 +2951,13 @@
         <v>41559</v>
       </c>
       <c r="B65">
-        <v>2.4708388251964402</v>
+        <v>2.46978498782395</v>
       </c>
       <c r="C65">
-        <v>32.562989343984299</v>
+        <v>32.558640914801202</v>
       </c>
       <c r="D65">
-        <v>7.0527229090255101</v>
+        <v>7.0508020962450999</v>
       </c>
       <c r="E65">
         <v>2.7598914464631399</v>
@@ -2971,13 +2971,13 @@
         <v>41587</v>
       </c>
       <c r="B66">
-        <v>2.44416161801594</v>
+        <v>2.4431924084305301</v>
       </c>
       <c r="C66">
-        <v>33.365169176914797</v>
+        <v>33.354727221749698</v>
       </c>
       <c r="D66">
-        <v>6.8254881165272803</v>
+        <v>6.8249564043680904</v>
       </c>
       <c r="E66">
         <v>2.25043870718588</v>
@@ -2991,13 +2991,13 @@
         <v>41615</v>
       </c>
       <c r="B67">
-        <v>2.4419767387065301</v>
+        <v>2.44106466612517</v>
       </c>
       <c r="C67">
-        <v>33.764507833087201</v>
+        <v>33.7546538261319</v>
       </c>
       <c r="D67">
-        <v>6.7445839262973504</v>
+        <v>6.7440702044562499</v>
       </c>
       <c r="E67">
         <v>2.2027106738423101</v>
@@ -3011,13 +3011,13 @@
         <v>41657</v>
       </c>
       <c r="B68">
-        <v>2.4232517296502301</v>
+        <v>2.4224248543090501</v>
       </c>
       <c r="C68">
-        <v>34.363646136840799</v>
+        <v>34.357170493691001</v>
       </c>
       <c r="D68">
-        <v>6.5872684846785097</v>
+        <v>6.5863281838438699</v>
       </c>
       <c r="E68">
         <v>2.3370415033488801</v>
@@ -3031,13 +3031,13 @@
         <v>41685</v>
       </c>
       <c r="B69">
-        <v>2.4086021481900799</v>
+        <v>2.4079229768288899</v>
       </c>
       <c r="C69">
-        <v>34.5090020990718</v>
+        <v>34.505098152838002</v>
       </c>
       <c r="D69">
-        <v>6.5242645000961002</v>
+        <v>6.5232346286975904</v>
       </c>
       <c r="E69">
         <v>2.1872679304828999</v>
@@ -3051,13 +3051,13 @@
         <v>41713</v>
       </c>
       <c r="B70">
-        <v>2.39860349243299</v>
+        <v>2.39785003866292</v>
       </c>
       <c r="C70">
-        <v>34.875079859729901</v>
+        <v>34.867966986916599</v>
       </c>
       <c r="D70">
-        <v>6.4351125961202102</v>
+        <v>6.4344491280494998</v>
       </c>
       <c r="E70">
         <v>2.2370420065448098</v>
@@ -3071,13 +3071,13 @@
         <v>41741</v>
       </c>
       <c r="B71">
-        <v>2.37801303289854</v>
+        <v>2.3773885033679401</v>
       </c>
       <c r="C71">
-        <v>35.3471916219805</v>
+        <v>35.337994499375803</v>
       </c>
       <c r="D71">
-        <v>6.30351261087457</v>
+        <v>6.3034982388883396</v>
       </c>
       <c r="E71">
         <v>2.38157621759269</v>
@@ -3091,13 +3091,13 @@
         <v>41776</v>
       </c>
       <c r="B72">
-        <v>2.3861491263112802</v>
+        <v>2.38551449802224</v>
       </c>
       <c r="C72">
-        <v>35.412737249227497</v>
+        <v>35.407276082181198</v>
       </c>
       <c r="D72">
-        <v>6.3127498059187603</v>
+        <v>6.3120887910082297</v>
       </c>
       <c r="E72">
         <v>2.4220073523794601</v>
@@ -3111,13 +3111,13 @@
         <v>41804</v>
       </c>
       <c r="B73">
-        <v>2.35050559492693</v>
+        <v>2.3500039265444101</v>
       </c>
       <c r="C73">
-        <v>35.968819562045603</v>
+        <v>35.9603855834809</v>
       </c>
       <c r="D73">
-        <v>6.1339952760082301</v>
+        <v>6.1341165062533198</v>
       </c>
       <c r="E73">
         <v>2.3201829275050598</v>
@@ -3131,13 +3131,13 @@
         <v>41832</v>
       </c>
       <c r="B74">
-        <v>2.3347895983659099</v>
+        <v>2.3343846270522399</v>
       </c>
       <c r="C74">
-        <v>36.515799951876801</v>
+        <v>36.511342392771198</v>
       </c>
       <c r="D74">
-        <v>6.00966323907772</v>
+        <v>6.0093729893663097</v>
       </c>
       <c r="E74">
         <v>2.4444104777984998</v>
@@ -3151,13 +3151,13 @@
         <v>41867</v>
       </c>
       <c r="B75">
-        <v>2.3227046415930399</v>
+        <v>2.32240921299924</v>
       </c>
       <c r="C75">
-        <v>37.019012586958603</v>
+        <v>37.015924708526498</v>
       </c>
       <c r="D75">
-        <v>5.9039228717433296</v>
+        <v>5.90367964650489</v>
       </c>
       <c r="E75">
         <v>2.4908643382169</v>
@@ -3171,13 +3171,13 @@
         <v>41895</v>
       </c>
       <c r="B76">
-        <v>2.3055538748847599</v>
+        <v>2.3052127690857498</v>
       </c>
       <c r="C76">
-        <v>37.246747238710803</v>
+        <v>37.237586307683202</v>
       </c>
       <c r="D76">
-        <v>5.8291270292040096</v>
+        <v>5.8296651297000404</v>
       </c>
       <c r="E76">
         <v>2.2593179013879601</v>
@@ -3191,13 +3191,13 @@
         <v>41930</v>
       </c>
       <c r="B77">
-        <v>2.29745112465831</v>
+        <v>2.2971952055848899</v>
       </c>
       <c r="C77">
-        <v>37.814791217007503</v>
+        <v>37.8065436568302</v>
       </c>
       <c r="D77">
-        <v>5.7275559543373697</v>
+        <v>5.7281322658366998</v>
       </c>
       <c r="E77">
         <v>2.3909410796341799</v>
@@ -3211,13 +3211,13 @@
         <v>41958</v>
       </c>
       <c r="B78">
-        <v>2.2984390896466702</v>
+        <v>2.2981827029665598</v>
       </c>
       <c r="C78">
-        <v>38.001893510954403</v>
+        <v>37.997044209635099</v>
       </c>
       <c r="D78">
-        <v>5.70327573329355</v>
+        <v>5.7033621077533603</v>
       </c>
       <c r="E78">
         <v>2.3242809771505399</v>
@@ -3231,13 +3231,13 @@
         <v>41986</v>
       </c>
       <c r="B79">
-        <v>2.2810680259508498</v>
+        <v>2.28084322855244</v>
       </c>
       <c r="C79">
-        <v>38.507109231255598</v>
+        <v>38.497909275418003</v>
       </c>
       <c r="D79">
-        <v>5.5924735532226704</v>
+        <v>5.5932148202188499</v>
       </c>
       <c r="E79">
         <v>2.2892033177678899</v>
@@ -3251,13 +3251,13 @@
         <v>42021</v>
       </c>
       <c r="B80">
-        <v>2.27528211948571</v>
+        <v>2.2752365572706301</v>
       </c>
       <c r="C80">
-        <v>39.424028033483502</v>
+        <v>39.422023045986101</v>
       </c>
       <c r="D80">
-        <v>5.4564023029136299</v>
+        <v>5.4565613637902404</v>
       </c>
       <c r="E80">
         <v>2.2037818012792201</v>
@@ -3271,13 +3271,13 @@
         <v>42049</v>
       </c>
       <c r="B81">
-        <v>2.26118050409886</v>
+        <v>2.2611673045322598</v>
       </c>
       <c r="C81">
-        <v>39.311781776121897</v>
+        <v>39.3101503204945</v>
       </c>
       <c r="D81">
-        <v>5.4390651521473696</v>
+        <v>5.43924858222677</v>
       </c>
       <c r="E81">
         <v>2.31141040965008</v>
@@ -3291,13 +3291,13 @@
         <v>42077</v>
       </c>
       <c r="B82">
-        <v>2.25577008916706</v>
+        <v>2.2557570765273001</v>
       </c>
       <c r="C82">
-        <v>39.689312541773901</v>
+        <v>39.682963254462102</v>
       </c>
       <c r="D82">
-        <v>5.3779130893953404</v>
+        <v>5.37869791620819</v>
       </c>
       <c r="E82">
         <v>2.3387126334017698</v>
@@ -3311,13 +3311,13 @@
         <v>42112</v>
       </c>
       <c r="B83">
-        <v>2.2648093024882501</v>
+        <v>2.2647990786928598</v>
       </c>
       <c r="C83">
-        <v>39.282808321130801</v>
+        <v>39.285099139120099</v>
       </c>
       <c r="D83">
-        <v>5.4511171326481698</v>
+        <v>5.4507933252214604</v>
       </c>
       <c r="E83">
         <v>2.6290574486209999</v>
@@ -3331,13 +3331,13 @@
         <v>42140</v>
       </c>
       <c r="B84">
-        <v>2.2450232431138502</v>
+        <v>2.24502926668977</v>
       </c>
       <c r="C84">
-        <v>39.900636298917298</v>
+        <v>39.897452368267999</v>
       </c>
       <c r="D84">
-        <v>5.3268195764617898</v>
+        <v>5.3272355580206003</v>
       </c>
       <c r="E84">
         <v>2.27344648073964</v>
@@ -3351,13 +3351,13 @@
         <v>42168</v>
       </c>
       <c r="B85">
-        <v>2.22553862839528</v>
+        <v>2.2256581454033002</v>
       </c>
       <c r="C85">
-        <v>40.084971080420097</v>
+        <v>40.080598605657599</v>
       </c>
       <c r="D85">
-        <v>5.2600137500390201</v>
+        <v>5.260825032334</v>
       </c>
       <c r="E85">
         <v>2.2679755088834801</v>
@@ -3371,13 +3371,13 @@
         <v>42203</v>
       </c>
       <c r="B86">
-        <v>2.2354551457821898</v>
+        <v>2.2354626686288399</v>
       </c>
       <c r="C86">
-        <v>40.0659414772907</v>
+        <v>40.062120506263497</v>
       </c>
       <c r="D86">
-        <v>5.2845894562329399</v>
+        <v>5.2850836876084299</v>
       </c>
       <c r="E86">
         <v>2.5108082424949401</v>
@@ -3391,13 +3391,13 @@
         <v>42231</v>
       </c>
       <c r="B87">
-        <v>2.21922890793673</v>
+        <v>2.21945872062147</v>
       </c>
       <c r="C87">
-        <v>41.165873343533697</v>
+        <v>41.163450447827003</v>
       </c>
       <c r="D87">
-        <v>5.11518653355603</v>
+        <v>5.1159748462319401</v>
       </c>
       <c r="E87">
         <v>1.93320930795823</v>
@@ -3411,13 +3411,13 @@
         <v>42259</v>
       </c>
       <c r="B88">
-        <v>2.2049080528260299</v>
+        <v>2.2051523025859501</v>
       </c>
       <c r="C88">
-        <v>41.500734894397901</v>
+        <v>41.497227812300402</v>
       </c>
       <c r="D88">
-        <v>5.0449047403067198</v>
+        <v>5.0458402878492397</v>
       </c>
       <c r="E88">
         <v>2.2863466789298399</v>
@@ -3431,13 +3431,13 @@
         <v>42294</v>
       </c>
       <c r="B89">
-        <v>2.2159544099118098</v>
+        <v>2.2160649264707901</v>
       </c>
       <c r="C89">
-        <v>41.122825698078103</v>
+        <v>41.122845245190099</v>
       </c>
       <c r="D89">
-        <v>5.1130982560888398</v>
+        <v>5.1133379166508499</v>
       </c>
       <c r="E89">
         <v>2.25110510217857</v>
@@ -3451,13 +3451,13 @@
         <v>42322</v>
       </c>
       <c r="B90">
-        <v>2.2133905119438202</v>
+        <v>2.21352529221409</v>
       </c>
       <c r="C90">
-        <v>41.193642004689003</v>
+        <v>41.190892534343597</v>
       </c>
       <c r="D90">
-        <v>5.0991518738252504</v>
+        <v>5.0997695696766501</v>
       </c>
       <c r="E90">
         <v>2.2491553319552402</v>
@@ -3471,13 +3471,13 @@
         <v>42350</v>
       </c>
       <c r="B91">
-        <v>2.1960650808257198</v>
+        <v>2.1963699351252401</v>
       </c>
       <c r="C91">
-        <v>42.244372078879699</v>
+        <v>42.240701877977102</v>
       </c>
       <c r="D91">
-        <v>4.9415919850962098</v>
+        <v>4.9426522619738398</v>
       </c>
       <c r="E91">
         <v>2.2824964755458099</v>
@@ -3491,13 +3491,13 @@
         <v>42385</v>
       </c>
       <c r="B92">
-        <v>2.2211229019502299</v>
+        <v>2.2213843045255</v>
       </c>
       <c r="C92">
-        <v>41.849900839098098</v>
+        <v>41.850733582631001</v>
       </c>
       <c r="D92">
-        <v>5.0398713562931103</v>
+        <v>5.0403393597130899</v>
       </c>
       <c r="E92">
         <v>2.0525912047455002</v>
@@ -3511,13 +3511,13 @@
         <v>42413</v>
       </c>
       <c r="B93">
-        <v>2.1977979533341401</v>
+        <v>2.1980406201485501</v>
       </c>
       <c r="C93">
-        <v>41.848436118841001</v>
+        <v>41.847844937013903</v>
       </c>
       <c r="D93">
-        <v>4.9897522447271596</v>
+        <v>4.9903426672985196</v>
       </c>
       <c r="E93">
         <v>2.0749409565136099</v>
@@ -3531,13 +3531,13 @@
         <v>42441</v>
       </c>
       <c r="B94">
-        <v>2.1912929085817199</v>
+        <v>2.19153042265149</v>
       </c>
       <c r="C94">
-        <v>42.2095729406186</v>
+        <v>42.207120447834001</v>
       </c>
       <c r="D94">
-        <v>4.93524814588989</v>
+        <v>4.9360293154950998</v>
       </c>
       <c r="E94">
         <v>2.2374746344530299</v>
@@ -3551,13 +3551,13 @@
         <v>42476</v>
       </c>
       <c r="B95">
-        <v>2.1871796888686998</v>
+        <v>2.18747810072828</v>
       </c>
       <c r="C95">
-        <v>42.136793629875498</v>
+        <v>42.136833859531002</v>
       </c>
       <c r="D95">
-        <v>4.93452983815365</v>
+        <v>4.9351653843821603</v>
       </c>
       <c r="E95">
         <v>2.4777673804621201</v>
@@ -3571,13 +3571,13 @@
         <v>42504</v>
       </c>
       <c r="B96">
-        <v>2.19806704870168</v>
+        <v>2.19835504234279</v>
       </c>
       <c r="C96">
-        <v>41.889528004799502</v>
+        <v>41.886943986564297</v>
       </c>
       <c r="D96">
-        <v>4.9856814508350498</v>
+        <v>4.9865943767361296</v>
       </c>
       <c r="E96">
         <v>2.1929470637644899</v>
@@ -3591,13 +3591,13 @@
         <v>42539</v>
       </c>
       <c r="B97">
-        <v>2.1861961651759301</v>
+        <v>2.1864532322076502</v>
       </c>
       <c r="C97">
-        <v>42.090177996630999</v>
+        <v>42.089146543274602</v>
       </c>
       <c r="D97">
-        <v>4.9376133582811796</v>
+        <v>4.9382803243659499</v>
       </c>
       <c r="E97">
         <v>2.2588736776132801</v>
@@ -3611,13 +3611,13 @@
         <v>42567</v>
       </c>
       <c r="B98">
-        <v>2.17471030817092</v>
+        <v>2.1750704231788802</v>
       </c>
       <c r="C98">
-        <v>42.684225539402803</v>
+        <v>42.681246325939703</v>
       </c>
       <c r="D98">
-        <v>4.8478865293647999</v>
+        <v>4.84897240971444</v>
       </c>
       <c r="E98">
         <v>2.06030617977714</v>
@@ -3631,13 +3631,13 @@
         <v>42595</v>
       </c>
       <c r="B99">
-        <v>2.1697234780285002</v>
+        <v>2.1701689875091201</v>
       </c>
       <c r="C99">
-        <v>42.9849080315999</v>
+        <v>42.984105104361703</v>
       </c>
       <c r="D99">
-        <v>4.8050961894481397</v>
+        <v>4.8061208626534402</v>
       </c>
       <c r="E99">
         <v>2.1064196622028701</v>
@@ -3651,13 +3651,13 @@
         <v>42630</v>
       </c>
       <c r="B100">
-        <v>2.16863885507993</v>
+        <v>2.1689544172327402</v>
       </c>
       <c r="C100">
-        <v>42.954234713841402</v>
+        <v>42.952370155714704</v>
       </c>
       <c r="D100">
-        <v>4.80607435554281</v>
+        <v>4.8069387097140703</v>
       </c>
       <c r="E100">
         <v>2.4690095503220402</v>
@@ -3671,13 +3671,13 @@
         <v>42658</v>
       </c>
       <c r="B101">
-        <v>2.1647012951773799</v>
+        <v>2.1651096105996301</v>
       </c>
       <c r="C101">
-        <v>43.228806806103201</v>
+        <v>43.221919526294798</v>
       </c>
       <c r="D101">
-        <v>4.7687464259152703</v>
+        <v>4.7703267910955898</v>
       </c>
       <c r="E101">
         <v>2.3313118604690501</v>
@@ -3691,13 +3691,13 @@
         <v>42686</v>
       </c>
       <c r="B102">
-        <v>2.13748637028716</v>
+        <v>2.1379267866162999</v>
       </c>
       <c r="C102">
-        <v>44.108118721535</v>
+        <v>44.098952029894399</v>
       </c>
       <c r="D102">
-        <v>4.6220313606949404</v>
+        <v>4.6238561973453596</v>
       </c>
       <c r="E102">
         <v>2.3301389046133298</v>
@@ -3711,13 +3711,13 @@
         <v>42714</v>
       </c>
       <c r="B103">
-        <v>2.1589373257442501</v>
+        <v>2.1592461247002701</v>
       </c>
       <c r="C103">
-        <v>43.650588754319003</v>
+        <v>43.643290546194599</v>
       </c>
       <c r="D103">
-        <v>4.7128567144985896</v>
+        <v>4.7142500866602903</v>
       </c>
       <c r="E103">
         <v>2.2301228508984901</v>
@@ -3731,13 +3731,13 @@
         <v>42749</v>
       </c>
       <c r="B104">
-        <v>2.14521765957595</v>
+        <v>2.1457432977187501</v>
       </c>
       <c r="C104">
-        <v>44.012574627160603</v>
+        <v>44.011956632551197</v>
       </c>
       <c r="D104">
-        <v>4.64757423026139</v>
+        <v>4.6487223171005096</v>
       </c>
       <c r="E104">
         <v>2.32811877253013</v>
@@ -3751,13 +3751,13 @@
         <v>42784</v>
       </c>
       <c r="B105">
-        <v>2.1327669872809398</v>
+        <v>2.1332844982394699</v>
       </c>
       <c r="C105">
-        <v>44.510436078295797</v>
+        <v>44.507235304366802</v>
       </c>
       <c r="D105">
-        <v>4.5725139936947103</v>
+        <v>4.5738866274819197</v>
       </c>
       <c r="E105">
         <v>2.4382074044990798</v>
@@ -3771,13 +3771,13 @@
         <v>42812</v>
       </c>
       <c r="B106">
-        <v>2.1249772178116602</v>
+        <v>2.1255128480329399</v>
       </c>
       <c r="C106">
-        <v>45.193263875349402</v>
+        <v>45.189322193678301</v>
       </c>
       <c r="D106">
-        <v>4.49082038706376</v>
+        <v>4.4922757231619999</v>
       </c>
       <c r="E106">
         <v>2.2602922291891701</v>
@@ -3791,13 +3791,13 @@
         <v>42840</v>
       </c>
       <c r="B107">
-        <v>2.11054117985663</v>
+        <v>2.1111548561335098</v>
       </c>
       <c r="C107">
-        <v>45.509869621945299</v>
+        <v>45.507585954094402</v>
       </c>
       <c r="D107">
-        <v>4.4320096032786997</v>
+        <v>4.4334537625574102</v>
       </c>
       <c r="E107">
         <v>2.2063028347273299</v>
@@ -3811,13 +3811,13 @@
         <v>42868</v>
       </c>
       <c r="B108">
-        <v>2.1003130442667901</v>
+        <v>2.1009159851644199</v>
       </c>
       <c r="C108">
-        <v>45.928751138926302</v>
+        <v>45.925363391662799</v>
       </c>
       <c r="D108">
-        <v>4.3730043047596103</v>
+        <v>4.3745133131801897</v>
       </c>
       <c r="E108">
         <v>1.9929901042212901</v>
@@ -3831,13 +3831,13 @@
         <v>42903</v>
       </c>
       <c r="B109">
-        <v>2.1031443702577599</v>
+        <v>2.1038619288364</v>
       </c>
       <c r="C109">
-        <v>46.265565707728499</v>
+        <v>46.266646453257401</v>
       </c>
       <c r="D109">
-        <v>4.34815062644177</v>
+        <v>4.34947243518166</v>
       </c>
       <c r="E109">
         <v>2.24543129961768</v>
@@ -3851,13 +3851,13 @@
         <v>42931</v>
       </c>
       <c r="B110">
-        <v>2.1030947395882502</v>
+        <v>2.1038262006090398</v>
       </c>
       <c r="C110">
-        <v>46.426190544745801</v>
+        <v>46.431137031669202</v>
       </c>
       <c r="D110">
-        <v>4.33366106108131</v>
+        <v>4.3346611607400796</v>
       </c>
       <c r="E110">
         <v>1.9195272742624101</v>
@@ -3871,13 +3871,13 @@
         <v>42959</v>
       </c>
       <c r="B111">
-        <v>2.10171262060565</v>
+        <v>2.1024438499289801</v>
       </c>
       <c r="C111">
-        <v>46.278086606221102</v>
+        <v>46.283658686974498</v>
       </c>
       <c r="D111">
-        <v>4.3441945898779997</v>
+        <v>4.3451399052557997</v>
       </c>
       <c r="E111">
         <v>2.1000398782148899</v>
@@ -3891,13 +3891,13 @@
         <v>42994</v>
       </c>
       <c r="B112">
-        <v>2.11059054238576</v>
+        <v>2.1112551019636299</v>
       </c>
       <c r="C112">
-        <v>46.008761005464002</v>
+        <v>46.012016452747403</v>
       </c>
       <c r="D112">
-        <v>4.3861574906864496</v>
+        <v>4.3871811573811197</v>
       </c>
       <c r="E112">
         <v>2.14473972451413</v>
@@ -3911,13 +3911,13 @@
         <v>43022</v>
       </c>
       <c r="B113">
-        <v>2.0776474271055498</v>
+        <v>2.0785155813993801</v>
       </c>
       <c r="C113">
-        <v>47.610397771425802</v>
+        <v>47.614009204277203</v>
       </c>
       <c r="D113">
-        <v>4.1813829036827599</v>
+        <v>4.1827530204271204</v>
       </c>
       <c r="E113">
         <v>2.0416755992300701</v>
@@ -3931,13 +3931,13 @@
         <v>43050</v>
       </c>
       <c r="B114">
-        <v>2.0907267475217801</v>
+        <v>2.0915886863087101</v>
       </c>
       <c r="C114">
-        <v>47.674104483475901</v>
+        <v>47.678298646789699</v>
       </c>
       <c r="D114">
-        <v>4.2012133786148604</v>
+        <v>4.2025184270765896</v>
       </c>
       <c r="E114">
         <v>2.1606430186436301</v>
@@ -3951,13 +3951,13 @@
         <v>43078</v>
       </c>
       <c r="B115">
-        <v>2.0781907761220602</v>
+        <v>2.0789849811447598</v>
       </c>
       <c r="C115">
-        <v>48.124049170861703</v>
+        <v>48.123338056159398</v>
       </c>
       <c r="D115">
-        <v>4.1396375506685397</v>
+        <v>4.1412127076269201</v>
       </c>
       <c r="E115">
         <v>2.1616102857982402</v>
@@ -3971,13 +3971,13 @@
         <v>43113</v>
       </c>
       <c r="B116">
-        <v>2.0750801815245499</v>
+        <v>2.0759980826986402</v>
       </c>
       <c r="C116">
-        <v>48.108907016728402</v>
+        <v>48.113835639755003</v>
       </c>
       <c r="D116">
-        <v>4.1349448247842497</v>
+        <v>4.1362920112044401</v>
       </c>
       <c r="E116">
         <v>2.13148664017316</v>
@@ -3991,13 +3991,13 @@
         <v>43148</v>
       </c>
       <c r="B117">
-        <v>2.0687084405920602</v>
+        <v>2.06962165016171</v>
       </c>
       <c r="C117">
-        <v>48.643347607030599</v>
+        <v>48.651317374797301</v>
       </c>
       <c r="D117">
-        <v>4.0793227524622102</v>
+        <v>4.0804087817524097</v>
       </c>
       <c r="E117">
         <v>2.3899286642648101</v>
@@ -4011,13 +4011,13 @@
         <v>43176</v>
       </c>
       <c r="B118">
-        <v>2.06180551775673</v>
+        <v>2.0627268177522802</v>
       </c>
       <c r="C118">
-        <v>49.112604957451602</v>
+        <v>49.114715703850301</v>
       </c>
       <c r="D118">
-        <v>4.0289775663474998</v>
+        <v>4.0305390736975104</v>
       </c>
       <c r="E118">
         <v>2.2391091023436398</v>
@@ -4031,13 +4031,13 @@
         <v>43204</v>
       </c>
       <c r="B119">
-        <v>2.0637490030325898</v>
+        <v>2.06474000240642</v>
       </c>
       <c r="C119">
-        <v>48.605823314444997</v>
+        <v>48.6126324805306</v>
       </c>
       <c r="D119">
-        <v>4.0729552444253398</v>
+        <v>4.0742838494667701</v>
       </c>
       <c r="E119">
         <v>2.0198618174921799</v>
@@ -4051,13 +4051,13 @@
         <v>43232</v>
       </c>
       <c r="B120">
-        <v>2.0341528013293799</v>
+        <v>2.0351629051313198</v>
       </c>
       <c r="C120">
-        <v>49.939798625398701</v>
+        <v>49.943565175600099</v>
       </c>
       <c r="D120">
-        <v>3.9137928625594101</v>
+        <v>3.9153765016534798</v>
       </c>
       <c r="E120">
         <v>1.8995298174861901</v>
@@ -4071,13 +4071,13 @@
         <v>43267</v>
       </c>
       <c r="B121">
-        <v>2.01548216501741</v>
+        <v>2.0165525344563902</v>
       </c>
       <c r="C121">
-        <v>50.755448374397297</v>
+        <v>50.759300127159598</v>
       </c>
       <c r="D121">
-        <v>3.8193038182490402</v>
+        <v>3.8209757545481202</v>
       </c>
       <c r="E121">
         <v>2.1242442691474599</v>
@@ -4091,13 +4091,13 @@
         <v>43295</v>
       </c>
       <c r="B122">
-        <v>2.0081031720579201</v>
+        <v>2.0091823680901402</v>
       </c>
       <c r="C122">
-        <v>50.9584291048712</v>
+        <v>50.961854362666699</v>
       </c>
       <c r="D122">
-        <v>3.79126796815543</v>
+        <v>3.7929829055498501</v>
       </c>
       <c r="E122">
         <v>1.85615798186308</v>
@@ -4111,13 +4111,13 @@
         <v>43330</v>
       </c>
       <c r="B123">
-        <v>1.99559147817657</v>
+        <v>1.99667604393551</v>
       </c>
       <c r="C123">
-        <v>51.571797860820801</v>
+        <v>51.573948283379103</v>
       </c>
       <c r="D123">
-        <v>3.7253849829186398</v>
+        <v>3.72718456991633</v>
       </c>
       <c r="E123">
         <v>2.19084591008497</v>
@@ -4131,13 +4131,13 @@
         <v>43358</v>
       </c>
       <c r="B124">
-        <v>1.99043470867808</v>
+        <v>1.9915101818237699</v>
       </c>
       <c r="C124">
-        <v>51.947324570724703</v>
+        <v>51.947950244800701</v>
       </c>
       <c r="D124">
-        <v>3.6902435979356101</v>
+        <v>3.6921210669744902</v>
       </c>
       <c r="E124">
         <v>1.9683604723519099</v>
@@ -4151,13 +4151,13 @@
         <v>43386</v>
       </c>
       <c r="B125">
-        <v>1.98887964253186</v>
+        <v>1.9899958534672</v>
       </c>
       <c r="C125">
-        <v>51.9861137346278</v>
+        <v>51.989145615057502</v>
       </c>
       <c r="D125">
-        <v>3.68481683477795</v>
+        <v>3.6866015266796501</v>
       </c>
       <c r="E125">
         <v>1.8928141943771599</v>
@@ -4171,13 +4171,13 @@
         <v>43414</v>
       </c>
       <c r="B126">
-        <v>2.0015226054024899</v>
+        <v>2.00272176590037</v>
       </c>
       <c r="C126">
-        <v>52.265394449010699</v>
+        <v>52.272165452222502</v>
       </c>
       <c r="D126">
-        <v>3.6882924515420199</v>
+        <v>3.6899602533520199</v>
       </c>
       <c r="E126">
         <v>2.07810181947473</v>
@@ -4191,13 +4191,13 @@
         <v>43442</v>
       </c>
       <c r="B127">
-        <v>2.0105746698602101</v>
+        <v>2.0116542543553799</v>
       </c>
       <c r="C127">
-        <v>51.799399469506497</v>
+        <v>51.806400776523802</v>
       </c>
       <c r="D127">
-        <v>3.7364349305443998</v>
+        <v>3.7378798865941101</v>
       </c>
       <c r="E127">
         <v>1.96634784208719</v>
@@ -4211,13 +4211,13 @@
         <v>43477</v>
       </c>
       <c r="B128">
-        <v>2.0225126662093098</v>
+        <v>2.0236553722150399</v>
       </c>
       <c r="C128">
-        <v>51.363928953799601</v>
+        <v>51.370646640758501</v>
       </c>
       <c r="D128">
-        <v>3.7884387961367501</v>
+        <v>3.7900212118576699</v>
       </c>
       <c r="E128">
         <v>2.2336276043318799</v>
@@ -4231,13 +4231,13 @@
         <v>43512</v>
       </c>
       <c r="B129">
-        <v>2.01408100252916</v>
+        <v>2.01527231133519</v>
       </c>
       <c r="C129">
-        <v>51.620990686364003</v>
+        <v>51.6239792795608</v>
       </c>
       <c r="D129">
-        <v>3.7551567269485799</v>
+        <v>3.75708506655831</v>
       </c>
       <c r="E129">
         <v>2.2243074163949701</v>
@@ -4251,13 +4251,13 @@
         <v>43540</v>
       </c>
       <c r="B130">
-        <v>2.0200283048944798</v>
+        <v>2.0210513406964701</v>
       </c>
       <c r="C130">
-        <v>50.867976508736703</v>
+        <v>50.869771429735501</v>
       </c>
       <c r="D130">
-        <v>3.8194450934814701</v>
+        <v>3.8211758388949102</v>
       </c>
       <c r="E130">
         <v>2.05694532224482</v>
@@ -4271,13 +4271,13 @@
         <v>43568</v>
       </c>
       <c r="B131">
-        <v>1.98145949472998</v>
+        <v>1.9826569507030301</v>
       </c>
       <c r="C131">
-        <v>52.216300005018397</v>
+        <v>52.217061526654199</v>
       </c>
       <c r="D131">
-        <v>3.6559804556850399</v>
+        <v>3.6580576549144102</v>
       </c>
       <c r="E131">
         <v>1.8758906761548899</v>
@@ -4291,13 +4291,13 @@
         <v>43603</v>
       </c>
       <c r="B132">
-        <v>1.99074704721439</v>
+        <v>1.9919580083936499</v>
       </c>
       <c r="C132">
-        <v>52.506126887907499</v>
+        <v>52.517342846271298</v>
       </c>
       <c r="D132">
-        <v>3.6529564055075099</v>
+        <v>3.6543451799256998</v>
       </c>
       <c r="E132">
         <v>2.0199627130878</v>
@@ -4311,13 +4311,13 @@
         <v>43631</v>
       </c>
       <c r="B133">
-        <v>1.9938350325870799</v>
+        <v>1.9950087203306499</v>
       </c>
       <c r="C133">
-        <v>51.826694094953801</v>
+        <v>51.833334733517098</v>
       </c>
       <c r="D133">
-        <v>3.7045994621535701</v>
+        <v>3.7062420879460301</v>
       </c>
       <c r="E133">
         <v>1.73103126528387</v>
@@ -4331,13 +4331,13 @@
         <v>43659</v>
       </c>
       <c r="B134">
-        <v>1.98673049787552</v>
+        <v>1.98790641911414</v>
       </c>
       <c r="C134">
-        <v>52.3961006941786</v>
+        <v>52.400771109919603</v>
       </c>
       <c r="D134">
-        <v>3.65323109210577</v>
+        <v>3.6550004696344298</v>
       </c>
       <c r="E134">
         <v>1.96289559154824</v>
@@ -4351,13 +4351,13 @@
         <v>43694</v>
       </c>
       <c r="B135">
-        <v>1.98108646425187</v>
+        <v>1.98231674174286</v>
       </c>
       <c r="C135">
-        <v>53.149533051341699</v>
+        <v>53.155394372424297</v>
       </c>
       <c r="D135">
-        <v>3.59344132472794</v>
+        <v>3.5952104316378102</v>
       </c>
       <c r="E135">
         <v>2.21792298413185</v>
@@ -4371,13 +4371,13 @@
         <v>43722</v>
       </c>
       <c r="B136">
-        <v>1.97535581337391</v>
+        <v>1.97652703608554</v>
       </c>
       <c r="C136">
-        <v>52.714009429813203</v>
+        <v>52.717131667813398</v>
       </c>
       <c r="D136">
-        <v>3.6119560075164499</v>
+        <v>3.6138138916361102</v>
       </c>
       <c r="E136">
         <v>1.7160474351658499</v>
@@ -4391,13 +4391,13 @@
         <v>43750</v>
       </c>
       <c r="B137">
-        <v>1.98511925312459</v>
+        <v>1.9863521107790101</v>
       </c>
       <c r="C137">
-        <v>52.786952975327402</v>
+        <v>52.798791724839802</v>
       </c>
       <c r="D137">
-        <v>3.6243274580606499</v>
+        <v>3.6257130523176202</v>
       </c>
       <c r="E137">
         <v>1.7460733008985001</v>
@@ -4411,13 +4411,13 @@
         <v>43778</v>
       </c>
       <c r="B138">
-        <v>2.0027096451827102</v>
+        <v>2.00385614171925</v>
       </c>
       <c r="C138">
-        <v>51.959357579071302</v>
+        <v>51.965230818444603</v>
       </c>
       <c r="D138">
-        <v>3.7113286206399598</v>
+        <v>3.7129702475759001</v>
       </c>
       <c r="E138">
         <v>1.9422352355063399</v>
@@ -4431,13 +4431,13 @@
         <v>43806</v>
       </c>
       <c r="B139">
-        <v>2.0117757762420201</v>
+        <v>2.0129567172385001</v>
       </c>
       <c r="C139">
-        <v>52.140169952332897</v>
+        <v>52.147735312239803</v>
       </c>
       <c r="D139">
-        <v>3.7150572323395599</v>
+        <v>3.71663773450845</v>
       </c>
       <c r="E139">
         <v>1.9695550817699901</v>
@@ -4451,13 +4451,13 @@
         <v>43848</v>
       </c>
       <c r="B140">
-        <v>2.0074659001884001</v>
+        <v>2.0091099659964899</v>
       </c>
       <c r="C140">
-        <v>52.638377858182601</v>
+        <v>52.6313586941992</v>
       </c>
       <c r="D140">
-        <v>3.6735930166342801</v>
+        <v>3.67696327513399</v>
       </c>
       <c r="E140">
         <v>1.9264905991547701</v>
@@ -4471,13 +4471,13 @@
         <v>43876</v>
       </c>
       <c r="B141">
-        <v>1.99870078249979</v>
+        <v>2.0001817810432501</v>
       </c>
       <c r="C141">
-        <v>52.252408079668903</v>
+        <v>52.259859137299799</v>
       </c>
       <c r="D141">
-        <v>3.6841657699158299</v>
+        <v>3.6862887443328001</v>
       </c>
       <c r="E141">
         <v>1.9979636987280001</v>
@@ -4491,13 +4491,13 @@
         <v>43904</v>
       </c>
       <c r="B142">
-        <v>2.1126667419388698</v>
+        <v>2.11529765958025</v>
       </c>
       <c r="C142">
-        <v>51.606167221700801</v>
+        <v>51.630542146092701</v>
       </c>
       <c r="D142">
-        <v>3.9328231572726602</v>
+        <v>3.93574212856001</v>
       </c>
       <c r="E142">
         <v>3.3786208794442398</v>
@@ -4511,13 +4511,13 @@
         <v>43939</v>
       </c>
       <c r="B143">
-        <v>3.9958462980763501</v>
+        <v>4.0010543026932801</v>
       </c>
       <c r="C143">
-        <v>18.147076746247201</v>
+        <v>18.1980163254022</v>
       </c>
       <c r="D143">
-        <v>18.045703767645499</v>
+        <v>18.0235216587377</v>
       </c>
       <c r="E143">
         <v>12.5154983898629</v>
@@ -4531,13 +4531,13 @@
         <v>43967</v>
       </c>
       <c r="B144">
-        <v>3.85217044462035</v>
+        <v>3.8582266115974502</v>
       </c>
       <c r="C144">
-        <v>17.8777111085336</v>
+        <v>17.909813102676399</v>
       </c>
       <c r="D144">
-        <v>17.727526195655798</v>
+        <v>17.724272200162901</v>
       </c>
       <c r="E144">
         <v>3.7193551272279999</v>
@@ -4551,13 +4551,13 @@
         <v>43995</v>
       </c>
       <c r="B145">
-        <v>3.2963555743823401</v>
+        <v>3.3020963298505102</v>
       </c>
       <c r="C145">
-        <v>25.852704535656301</v>
+        <v>25.8747268083135</v>
       </c>
       <c r="D145">
-        <v>11.3086170255181</v>
+        <v>11.317532118605801</v>
       </c>
       <c r="E145">
         <v>2.7377488129820899</v>
@@ -4571,13 +4571,13 @@
         <v>44030</v>
       </c>
       <c r="B146">
-        <v>3.2064810820830401</v>
+        <v>3.2104639030352402</v>
       </c>
       <c r="C146">
-        <v>27.335464185889101</v>
+        <v>27.363208698643302</v>
       </c>
       <c r="D146">
-        <v>10.4986144593924</v>
+        <v>10.500746655012501</v>
       </c>
       <c r="E146">
         <v>2.97524921022683</v>
@@ -4591,13 +4591,13 @@
         <v>44058</v>
       </c>
       <c r="B147">
-        <v>3.0483423996915402</v>
+        <v>3.0527084735944001</v>
       </c>
       <c r="C147">
-        <v>30.167796607927301</v>
+        <v>30.196143930743801</v>
       </c>
       <c r="D147">
-        <v>9.1772929990217609</v>
+        <v>9.1813950041658892</v>
       </c>
       <c r="E147">
         <v>2.2185000599290201</v>
@@ -4611,13 +4611,13 @@
         <v>44086</v>
       </c>
       <c r="B148">
-        <v>2.9282860943241298</v>
+        <v>2.93163429936833</v>
       </c>
       <c r="C148">
-        <v>32.101911494110098</v>
+        <v>32.126668434073203</v>
       </c>
       <c r="D148">
-        <v>8.3593193756091004</v>
+        <v>8.3621683618240095</v>
       </c>
       <c r="E148">
         <v>2.4009560070505902</v>
@@ -4631,13 +4631,13 @@
         <v>44121</v>
       </c>
       <c r="B149">
-        <v>2.7597925874832199</v>
+        <v>2.7624875150524502</v>
       </c>
       <c r="C149">
-        <v>34.372081160359201</v>
+        <v>34.390148591155899</v>
       </c>
       <c r="D149">
-        <v>7.4324086261431503</v>
+        <v>7.4355087675483196</v>
       </c>
       <c r="E149">
         <v>2.3324458902705398</v>
@@ -4651,13 +4651,13 @@
         <v>44149</v>
       </c>
       <c r="B150">
-        <v>2.6636670336239701</v>
+        <v>2.66685224411049</v>
       </c>
       <c r="C150">
-        <v>36.041293017028302</v>
+        <v>36.062526517445797</v>
       </c>
       <c r="D150">
-        <v>6.8819785116380201</v>
+        <v>6.8858637277127404</v>
       </c>
       <c r="E150">
         <v>2.3005158835911499</v>
@@ -4671,13 +4671,13 @@
         <v>44177</v>
       </c>
       <c r="B151">
-        <v>2.7161112917896499</v>
+        <v>2.7179408633094102</v>
       </c>
       <c r="C151">
-        <v>34.6344061646423</v>
+        <v>34.666326047870797</v>
       </c>
       <c r="D151">
-        <v>7.2719509039142398</v>
+        <v>7.2702799543103396</v>
       </c>
       <c r="E151">
         <v>2.6900508796200802</v>
@@ -4691,13 +4691,13 @@
         <v>44212</v>
       </c>
       <c r="B152">
-        <v>2.6880939240695199</v>
+        <v>2.6906213421986398</v>
       </c>
       <c r="C152">
-        <v>35.7184295312899</v>
+        <v>35.739966433768402</v>
       </c>
       <c r="D152">
-        <v>6.9990555828202998</v>
+        <v>7.0012495200014797</v>
       </c>
       <c r="E152">
         <v>2.1134364610362701</v>
@@ -4711,13 +4711,13 @@
         <v>44240</v>
       </c>
       <c r="B153">
-        <v>2.61469111650251</v>
+        <v>2.6167236236306501</v>
       </c>
       <c r="C153">
-        <v>36.7738893836638</v>
+        <v>36.790095093371797</v>
       </c>
       <c r="D153">
-        <v>6.6381958509306198</v>
+        <v>6.6402813239568603</v>
       </c>
       <c r="E153">
         <v>1.9591434923736299</v>
@@ -4731,13 +4731,13 @@
         <v>44268</v>
       </c>
       <c r="B154">
-        <v>2.5275589015450901</v>
+        <v>2.5282563694874698</v>
       </c>
       <c r="C154">
-        <v>39.229228852141901</v>
+        <v>39.2465466385719</v>
       </c>
       <c r="D154">
-        <v>6.0530491867682601</v>
+        <v>6.0521084180809002</v>
       </c>
       <c r="E154">
         <v>1.9406518811604501</v>
@@ -4751,13 +4751,13 @@
         <v>44303</v>
       </c>
       <c r="B155">
-        <v>2.4284653905351301</v>
+        <v>2.4284813731342201</v>
       </c>
       <c r="C155">
-        <v>42.138418400322301</v>
+        <v>42.141226702762502</v>
       </c>
       <c r="D155">
-        <v>5.44903566049486</v>
+        <v>5.4487262267879704</v>
       </c>
       <c r="E155">
         <v>2.1795322162346999</v>
@@ -4771,13 +4771,13 @@
         <v>44331</v>
       </c>
       <c r="B156">
-        <v>2.37094040687251</v>
+        <v>2.3705808763073999</v>
       </c>
       <c r="C156">
-        <v>44.393542956117102</v>
+        <v>44.391076772469901</v>
       </c>
       <c r="D156">
-        <v>5.0699595855022803</v>
+        <v>5.0694970954892602</v>
       </c>
       <c r="E156">
         <v>1.8043650486395599</v>
@@ -4791,13 +4791,13 @@
         <v>44359</v>
       </c>
       <c r="B157">
-        <v>2.3052465835098501</v>
+        <v>2.3053289885816399</v>
       </c>
       <c r="C157">
-        <v>46.074510620867201</v>
+        <v>46.068348715442902</v>
       </c>
       <c r="D157">
-        <v>4.7648990336422896</v>
+        <v>4.7656682270197699</v>
       </c>
       <c r="E157">
         <v>1.7409409098886099</v>
@@ -4811,13 +4811,13 @@
         <v>44394</v>
       </c>
       <c r="B158">
-        <v>2.2698038247506198</v>
+        <v>2.26949497401402</v>
       </c>
       <c r="C158">
-        <v>46.838750626558003</v>
+        <v>46.836247257686402</v>
       </c>
       <c r="D158">
-        <v>4.6220131097549197</v>
+        <v>4.6216488558621904</v>
       </c>
       <c r="E158">
         <v>2.09949533997733</v>
@@ -4831,13 +4831,13 @@
         <v>44422</v>
       </c>
       <c r="B159">
-        <v>2.2223066280199899</v>
+        <v>2.22275166720474</v>
       </c>
       <c r="C159">
-        <v>48.399304790717103</v>
+        <v>48.409319986870997</v>
       </c>
       <c r="D159">
-        <v>4.3900353341921203</v>
+        <v>4.39000735026376</v>
       </c>
       <c r="E159">
         <v>1.90158663191348</v>
@@ -4851,13 +4851,13 @@
         <v>44457</v>
       </c>
       <c r="B160">
-        <v>2.2153793397821699</v>
+        <v>2.2152210263206999</v>
       </c>
       <c r="C160">
-        <v>47.787453821272301</v>
+        <v>47.795481125817801</v>
       </c>
       <c r="D160">
-        <v>4.4305076327308104</v>
+        <v>4.4294939502783501</v>
       </c>
       <c r="E160">
         <v>2.1824784670481598</v>
@@ -4871,13 +4871,13 @@
         <v>44485</v>
       </c>
       <c r="B161">
-        <v>2.1164361156822502</v>
+        <v>2.11607912294172</v>
       </c>
       <c r="C161">
-        <v>49.8526677637742</v>
+        <v>49.855894208235497</v>
       </c>
       <c r="D161">
-        <v>4.0724891477662801</v>
+        <v>4.0715774047246196</v>
       </c>
       <c r="E161">
         <v>1.9252697776277501</v>
@@ -4891,13 +4891,13 @@
         <v>44513</v>
       </c>
       <c r="B162">
-        <v>2.0509660837313799</v>
+        <v>2.0513560556532902</v>
       </c>
       <c r="C162">
-        <v>51.859982897263698</v>
+        <v>51.844381908028097</v>
       </c>
       <c r="D162">
-        <v>3.8043590819638502</v>
+        <v>3.8061563551381901</v>
       </c>
       <c r="E162">
         <v>1.8646527166593601</v>
@@ -4911,13 +4911,13 @@
         <v>44541</v>
       </c>
       <c r="B163">
-        <v>2.0028019127293901</v>
+        <v>2.0028052919049002</v>
       </c>
       <c r="C163">
-        <v>54.0591010222874</v>
+        <v>54.029992719835199</v>
       </c>
       <c r="D163">
-        <v>3.5724829302546199</v>
+        <v>3.5743446034682602</v>
       </c>
       <c r="E163">
         <v>1.88258695142137</v>
@@ -4931,13 +4931,13 @@
         <v>44576</v>
       </c>
       <c r="B164">
-        <v>2.0052199949595</v>
+        <v>2.0058690799749801</v>
       </c>
       <c r="C164">
-        <v>54.605830807912</v>
+        <v>54.570098649779297</v>
       </c>
       <c r="D164">
-        <v>3.5420999372401498</v>
+        <v>3.5454436936127798</v>
       </c>
       <c r="E164">
         <v>2.3444431631417499</v>
@@ -4951,13 +4951,13 @@
         <v>44604</v>
       </c>
       <c r="B165">
-        <v>1.9976444744694399</v>
+        <v>1.9976938820355801</v>
       </c>
       <c r="C165">
-        <v>54.308443738967</v>
+        <v>54.271215391323103</v>
       </c>
       <c r="D165">
-        <v>3.5478303285731299</v>
+        <v>3.5502623168518102</v>
       </c>
       <c r="E165">
         <v>1.98348998593215</v>
@@ -4971,13 +4971,13 @@
         <v>44632</v>
       </c>
       <c r="B166">
-        <v>1.94689819267079</v>
+        <v>1.94697960427616</v>
       </c>
       <c r="C166">
-        <v>57.249501881869399</v>
+        <v>57.195850967993898</v>
       </c>
       <c r="D166">
-        <v>3.2888793747917999</v>
+        <v>3.2919959789496902</v>
       </c>
       <c r="E166">
         <v>2.2485420880998399</v>
@@ -4991,13 +4991,13 @@
         <v>44667</v>
       </c>
       <c r="B167">
-        <v>1.9234841534829901</v>
+        <v>1.92424412481301</v>
       </c>
       <c r="C167">
-        <v>57.933318927802397</v>
+        <v>57.883020345227798</v>
       </c>
       <c r="D167">
-        <v>3.2134762541041502</v>
+        <v>3.2174086908404198</v>
       </c>
       <c r="E167">
         <v>2.2342347828846498</v>
@@ -5011,13 +5011,13 @@
         <v>44695</v>
       </c>
       <c r="B168">
-        <v>1.92331109000152</v>
+        <v>1.92337776775744</v>
       </c>
       <c r="C168">
-        <v>56.922433624402501</v>
+        <v>56.858351168212302</v>
       </c>
       <c r="D168">
-        <v>3.2683945106582102</v>
+        <v>3.2720673627217498</v>
       </c>
       <c r="E168">
         <v>1.87926047061506</v>
@@ -5031,13 +5031,13 @@
         <v>44730</v>
       </c>
       <c r="B169">
-        <v>1.928657384586</v>
+        <v>1.92907478537262</v>
       </c>
       <c r="C169">
-        <v>56.589387643933399</v>
+        <v>56.542972768076197</v>
       </c>
       <c r="D169">
-        <v>3.2958335905549201</v>
+        <v>3.2991401294939702</v>
       </c>
       <c r="E169">
         <v>2.21268667407187</v>
@@ -5051,13 +5051,13 @@
         <v>44758</v>
       </c>
       <c r="B170">
-        <v>1.9404332451323401</v>
+        <v>1.9407699033148</v>
       </c>
       <c r="C170">
-        <v>55.9192831551022</v>
+        <v>55.878197276302103</v>
       </c>
       <c r="D170">
-        <v>3.3536860632183698</v>
+        <v>3.3566319116108101</v>
       </c>
       <c r="E170">
         <v>2.0164290003549801</v>
@@ -5071,13 +5071,13 @@
         <v>44786</v>
       </c>
       <c r="B171">
-        <v>1.9372492409158599</v>
+        <v>1.93748961610518</v>
       </c>
       <c r="C171">
-        <v>55.284224812221503</v>
+        <v>55.242767859152998</v>
       </c>
       <c r="D171">
-        <v>3.3855283754432399</v>
+        <v>3.38838910780269</v>
       </c>
       <c r="E171">
         <v>2.0400810152089499</v>
@@ -5091,13 +5091,13 @@
         <v>44821</v>
       </c>
       <c r="B172">
-        <v>1.92700886346194</v>
+        <v>1.92749664907537</v>
       </c>
       <c r="C172">
-        <v>55.7638617757543</v>
+        <v>55.725480857585602</v>
       </c>
       <c r="D172">
-        <v>3.3402318982373398</v>
+        <v>3.34327337881669</v>
       </c>
       <c r="E172">
         <v>2.1363873768330102</v>
@@ -5111,13 +5111,13 @@
         <v>44849</v>
       </c>
       <c r="B173">
-        <v>1.9277207677703401</v>
+        <v>1.92828592021112</v>
       </c>
       <c r="C173">
-        <v>55.1430990630748</v>
+        <v>55.092800527189198</v>
       </c>
       <c r="D173">
-        <v>3.3777695387660498</v>
+        <v>3.3817067340340601</v>
       </c>
       <c r="E173">
         <v>2.0811849562225802</v>
@@ -5131,13 +5131,13 @@
         <v>44877</v>
       </c>
       <c r="B174">
-        <v>1.9490712299744599</v>
+        <v>1.9496859441490899</v>
       </c>
       <c r="C174">
-        <v>53.808570505647801</v>
+        <v>53.768881026704001</v>
       </c>
       <c r="D174">
-        <v>3.4956127434802302</v>
+        <v>3.4991674232558498</v>
       </c>
       <c r="E174">
         <v>2.1677943046031301</v>
@@ -5151,13 +5151,13 @@
         <v>44905</v>
       </c>
       <c r="B175">
-        <v>1.95139936362135</v>
+        <v>1.95228994494965</v>
       </c>
       <c r="C175">
-        <v>54.364378098054097</v>
+        <v>54.3172893366295</v>
       </c>
       <c r="D175">
-        <v>3.46510241281733</v>
+        <v>3.46953001937367</v>
       </c>
       <c r="E175">
         <v>2.1884229670259598</v>
@@ -5171,13 +5171,13 @@
         <v>44940</v>
       </c>
       <c r="B176">
-        <v>1.9516788631406199</v>
+        <v>1.9505621976871701</v>
       </c>
       <c r="C176">
-        <v>54.114321139405</v>
+        <v>54.126991081095099</v>
       </c>
       <c r="D176">
-        <v>3.4810381747440702</v>
+        <v>3.4783297124077501</v>
       </c>
       <c r="E176">
         <v>1.75675798330476</v>
@@ -5191,13 +5191,13 @@
         <v>44975</v>
       </c>
       <c r="B177">
-        <v>1.9649413708529</v>
+        <v>1.96430749021383</v>
       </c>
       <c r="C177">
-        <v>54.275170149317503</v>
+        <v>54.308945818970599</v>
       </c>
       <c r="D177">
-        <v>3.4938433046104</v>
+        <v>3.4906591936692499</v>
       </c>
       <c r="E177">
         <v>2.0930086234189802</v>
@@ -5211,13 +5211,13 @@
         <v>45003</v>
       </c>
       <c r="B178">
-        <v>1.9817967255484601</v>
+        <v>1.9807348611837901</v>
       </c>
       <c r="C178">
-        <v>53.765262768108499</v>
+        <v>53.7886873187432</v>
       </c>
       <c r="D178">
-        <v>3.5549798384862799</v>
+        <v>3.5516503197637701</v>
       </c>
       <c r="E178">
         <v>2.17311598265462</v>
@@ -5231,13 +5231,13 @@
         <v>45031</v>
       </c>
       <c r="B179">
-        <v>1.9941305973980601</v>
+        <v>1.9936433900875501</v>
       </c>
       <c r="C179">
-        <v>52.7571670006879</v>
+        <v>52.787729797628302</v>
       </c>
       <c r="D179">
-        <v>3.6421613457208202</v>
+        <v>3.6392723914679199</v>
       </c>
       <c r="E179">
         <v>1.7214643261367799</v>
@@ -5251,13 +5251,13 @@
         <v>45059</v>
       </c>
       <c r="B180">
-        <v>1.98952440215288</v>
+        <v>1.9889643779628201</v>
       </c>
       <c r="C180">
-        <v>52.156352320616001</v>
+        <v>52.181390512823</v>
       </c>
       <c r="D180">
-        <v>3.674378406207</v>
+        <v>3.6716842301897699</v>
       </c>
       <c r="E180">
         <v>1.8492384361002101</v>
@@ -5271,13 +5271,13 @@
         <v>45094</v>
       </c>
       <c r="B181">
-        <v>2.0107392798582899</v>
+        <v>2.0107201160141801</v>
       </c>
       <c r="C181">
-        <v>51.644938451672097</v>
+        <v>51.679461693216403</v>
       </c>
       <c r="D181">
-        <v>3.7474865007188098</v>
+        <v>3.7450424793839798</v>
       </c>
       <c r="E181">
         <v>1.9631575400624801</v>
@@ -5291,13 +5291,13 @@
         <v>45122</v>
       </c>
       <c r="B182">
-        <v>2.00126322059289</v>
+        <v>2.0013164689060701</v>
       </c>
       <c r="C182">
-        <v>51.655159798431903</v>
+        <v>51.668390074982298</v>
       </c>
       <c r="D182">
-        <v>3.72977382387811</v>
+        <v>3.7289499007591802</v>
       </c>
       <c r="E182">
         <v>1.83016817052655</v>
@@ -5311,13 +5311,13 @@
         <v>45150</v>
       </c>
       <c r="B183">
-        <v>2.01682352925451</v>
+        <v>2.01711681198138</v>
       </c>
       <c r="C183">
-        <v>50.405621509414601</v>
+        <v>50.417726656683101</v>
       </c>
       <c r="D183">
-        <v>3.8472519314328202</v>
+        <v>3.8469015611476398</v>
       </c>
       <c r="E183">
         <v>1.93886220672929</v>
@@ -5331,13 +5331,13 @@
         <v>45185</v>
       </c>
       <c r="B184">
-        <v>2.0040111279797199</v>
+        <v>2.0041725132974202</v>
       </c>
       <c r="C184">
-        <v>50.881873269636003</v>
+        <v>50.890554123212098</v>
       </c>
       <c r="D184">
-        <v>3.78931193229714</v>
+        <v>3.7889835920129</v>
       </c>
       <c r="E184">
         <v>1.8976962303309</v>
@@ -5351,13 +5351,13 @@
         <v>45213</v>
       </c>
       <c r="B185">
-        <v>1.99508026436876</v>
+        <v>1.99544493186889</v>
       </c>
       <c r="C185">
-        <v>50.736431445159603</v>
+        <v>50.747656130198699</v>
       </c>
       <c r="D185">
-        <v>3.7834687451379398</v>
+        <v>3.7833287988142201</v>
       </c>
       <c r="E185">
         <v>2.0975001099503001</v>
@@ -5371,13 +5371,13 @@
         <v>45241</v>
       </c>
       <c r="B186">
-        <v>2.0186568975006298</v>
+        <v>2.0186854243505499</v>
       </c>
       <c r="C186">
-        <v>49.462979276231998</v>
+        <v>49.487258796259702</v>
       </c>
       <c r="D186">
-        <v>3.92112032082346</v>
+        <v>3.9193251476064899</v>
       </c>
       <c r="E186">
         <v>1.8892248908972</v>
@@ -5391,13 +5391,13 @@
         <v>45269</v>
       </c>
       <c r="B187">
-        <v>2.0035241646402202</v>
+        <v>2.0047514932111601</v>
       </c>
       <c r="C187">
-        <v>50.254106820454901</v>
+        <v>50.272835613657499</v>
       </c>
       <c r="D187">
-        <v>3.8339360718660802</v>
+        <v>3.8348202435451699</v>
       </c>
       <c r="E187">
         <v>2.0503070770834699</v>
@@ -5411,13 +5411,13 @@
         <v>45304</v>
       </c>
       <c r="B188">
-        <v>1.97912014254475</v>
+        <v>1.98002572546359</v>
       </c>
       <c r="C188">
-        <v>51.568663680584599</v>
+        <v>51.571364492546003</v>
       </c>
       <c r="D188">
-        <v>3.6959888929892402</v>
+        <v>3.6974310422247498</v>
       </c>
       <c r="E188">
         <v>1.9888319505750101</v>
@@ -5431,13 +5431,13 @@
         <v>45339</v>
       </c>
       <c r="B189">
-        <v>1.99794487581062</v>
+        <v>1.99915176985711</v>
       </c>
       <c r="C189">
-        <v>50.985474158756801</v>
+        <v>51.004648737912603</v>
       </c>
       <c r="D189">
-        <v>3.7708870288403298</v>
+        <v>3.7717140105152702</v>
       </c>
       <c r="E189">
         <v>2.1003720353858899</v>
@@ -5451,13 +5451,13 @@
         <v>45367</v>
       </c>
       <c r="B190">
-        <v>2.0198194793926199</v>
+        <v>2.0206656378666099</v>
       </c>
       <c r="C190">
-        <v>50.5398540618406</v>
+        <v>50.5678582928943</v>
       </c>
       <c r="D190">
-        <v>3.84290720110365</v>
+        <v>3.8424079757915499</v>
       </c>
       <c r="E190">
         <v>1.9760772983664701</v>
@@ -5471,13 +5471,13 @@
         <v>45395</v>
       </c>
       <c r="B191">
-        <v>2.01025258014629</v>
+        <v>2.0106452239921802</v>
       </c>
       <c r="C191">
-        <v>49.609127174629002</v>
+        <v>49.630121546637199</v>
       </c>
       <c r="D191">
-        <v>3.89437569706622</v>
+        <v>3.89352317893105</v>
       </c>
       <c r="E191">
         <v>2.1196643458276898</v>
@@ -5491,13 +5491,13 @@
         <v>45430</v>
       </c>
       <c r="B192">
-        <v>2.0203408373068901</v>
+        <v>2.0207827233522302</v>
       </c>
       <c r="C192">
-        <v>49.284687535502997</v>
+        <v>49.315094140122298</v>
       </c>
       <c r="D192">
-        <v>3.9379002436681501</v>
+        <v>3.9363946752607499</v>
       </c>
       <c r="E192">
         <v>2.10109057734216</v>
@@ -5511,13 +5511,13 @@
         <v>45458</v>
       </c>
       <c r="B193">
-        <v>2.0438712131206</v>
+        <v>2.0447081381304399</v>
       </c>
       <c r="C193">
-        <v>47.994383848140899</v>
+        <v>47.990194412781598</v>
       </c>
       <c r="D193">
-        <v>4.0846172805552401</v>
+        <v>4.0865636463464501</v>
       </c>
       <c r="E193">
         <v>1.8885110943969401</v>
@@ -5531,13 +5531,13 @@
         <v>45486</v>
       </c>
       <c r="B194">
-        <v>2.0536524411935102</v>
+        <v>2.05525320602134</v>
       </c>
       <c r="C194">
-        <v>47.605997759396402</v>
+        <v>47.6008101813228</v>
       </c>
       <c r="D194">
-        <v>4.1354549073507503</v>
+        <v>4.1389773288898404</v>
       </c>
       <c r="E194">
         <v>2.0972827536666698</v>
@@ -5551,13 +5551,13 @@
         <v>45521</v>
       </c>
       <c r="B195">
-        <v>2.06094515609339</v>
+        <v>2.0616899391891899</v>
       </c>
       <c r="C195">
-        <v>46.959969822062398</v>
+        <v>46.960863018900497</v>
       </c>
       <c r="D195">
-        <v>4.2042160106798798</v>
+        <v>4.2055948023591698</v>
       </c>
       <c r="E195">
         <v>2.2473534047530199</v>
@@ -5571,13 +5571,13 @@
         <v>45549</v>
       </c>
       <c r="B196">
-        <v>2.0560523955623999</v>
+        <v>2.0567847213310202</v>
       </c>
       <c r="C196">
-        <v>46.482769326500197</v>
+        <v>46.483587735861299</v>
       </c>
       <c r="D196">
-        <v>4.2358926785152002</v>
+        <v>4.2372660472370498</v>
       </c>
       <c r="E196">
         <v>1.95870889634179</v>
@@ -5591,13 +5591,13 @@
         <v>45577</v>
       </c>
       <c r="B197">
-        <v>2.0661831856329398</v>
+        <v>2.0675195953243701</v>
       </c>
       <c r="C197">
-        <v>46.900312005349001</v>
+        <v>46.914516558149501</v>
       </c>
       <c r="D197">
-        <v>4.2195856117010102</v>
+        <v>4.2209751935307001</v>
       </c>
       <c r="E197">
         <v>1.86969713677436</v>
@@ -5611,13 +5611,13 @@
         <v>45605</v>
       </c>
       <c r="B198">
-        <v>2.05236800266557</v>
+        <v>2.05346626623392</v>
       </c>
       <c r="C198">
-        <v>47.781729874369098</v>
+        <v>47.788609171390597</v>
       </c>
       <c r="D198">
-        <v>4.1184010348291604</v>
+        <v>4.1199453437763802</v>
       </c>
       <c r="E198">
         <v>1.9386235268069101</v>
@@ -5631,13 +5631,13 @@
         <v>45633</v>
       </c>
       <c r="B199">
-        <v>2.0622303317547299</v>
+        <v>2.0629625247932499</v>
       </c>
       <c r="C199">
-        <v>47.370779396125698</v>
+        <v>47.373471950372803</v>
       </c>
       <c r="D199">
-        <v>4.17176769755054</v>
+        <v>4.1729597748995504</v>
       </c>
       <c r="E199">
         <v>1.9595128396592201</v>
@@ -5651,13 +5651,13 @@
         <v>45675</v>
       </c>
       <c r="B200">
-        <v>2.04709432728695</v>
+        <v>2.0486918466834898</v>
       </c>
       <c r="C200">
-        <v>47.532908658647699</v>
+        <v>47.532711058570499</v>
       </c>
       <c r="D200">
-        <v>4.1288709237627401</v>
+        <v>4.1319763593587098</v>
       </c>
       <c r="E200">
         <v>2.0185607882052499</v>
@@ -5671,13 +5671,13 @@
         <v>45703</v>
       </c>
       <c r="B201">
-        <v>2.0456879240591999</v>
+        <v>2.0472138135706501</v>
       </c>
       <c r="C201">
-        <v>47.599183135616201</v>
+        <v>47.603457909667299</v>
       </c>
       <c r="D201">
-        <v>4.1206430400437304</v>
+        <v>4.1232348778324699</v>
       </c>
       <c r="E201">
         <v>2.0578873333639001</v>
@@ -5691,13 +5691,13 @@
         <v>45731</v>
       </c>
       <c r="B202">
-        <v>2.0525957968848298</v>
+        <v>2.0539488848402101</v>
       </c>
       <c r="C202">
-        <v>47.119774168371698</v>
+        <v>47.127255974804498</v>
       </c>
       <c r="D202">
-        <v>4.1742868979776997</v>
+        <v>4.1762882603259799</v>
       </c>
       <c r="E202">
         <v>2.10667169363363</v>
@@ -5711,13 +5711,13 @@
         <v>45759</v>
       </c>
       <c r="B203">
-        <v>2.0484043684761999</v>
+        <v>2.0494694899581298</v>
       </c>
       <c r="C203">
-        <v>47.350828395154203</v>
+        <v>47.358541345380999</v>
       </c>
       <c r="D203">
-        <v>4.1466319492806099</v>
+        <v>4.1480510049035404</v>
       </c>
       <c r="E203">
         <v>1.9077452351988</v>
@@ -5731,13 +5731,13 @@
         <v>45794</v>
       </c>
       <c r="B204">
-        <v>2.06703755947597</v>
+        <v>2.06820472516916</v>
       </c>
       <c r="C204">
-        <v>46.146593952506102</v>
+        <v>46.155714125478099</v>
       </c>
       <c r="D204">
-        <v>4.2872471843616902</v>
+        <v>4.2887529144500496</v>
       </c>
       <c r="E204">
         <v>2.2144703593577599</v>
@@ -5751,13 +5751,13 @@
         <v>45822</v>
       </c>
       <c r="B205">
-        <v>2.0798657977638801</v>
+        <v>2.0804280566115598</v>
       </c>
       <c r="C205">
-        <v>45.837512539415499</v>
+        <v>45.846332799705401</v>
       </c>
       <c r="D205">
-        <v>4.3405250244045597</v>
+        <v>4.3408484517629304</v>
       </c>
       <c r="E205">
         <v>2.0284282924494401</v>
@@ -5771,13 +5771,13 @@
         <v>45850</v>
       </c>
       <c r="B206">
-        <v>2.0626599275192801</v>
+        <v>2.06243083947628</v>
       </c>
       <c r="C206">
-        <v>45.703026780817197</v>
+        <v>45.717916953401001</v>
       </c>
       <c r="D206">
-        <v>4.3182880215125001</v>
+        <v>4.3164835225074096</v>
       </c>
       <c r="E206">
         <v>2.0116722163937801</v>
@@ -5791,13 +5791,13 @@
         <v>45885</v>
       </c>
       <c r="B207">
-        <v>2.0814367705456398</v>
+        <v>2.0816207813875098</v>
       </c>
       <c r="C207">
-        <v>45.528497720606701</v>
+        <v>45.546833830089298</v>
       </c>
       <c r="D207">
-        <v>4.3718538846812596</v>
+        <v>4.3705402544929699</v>
       </c>
       <c r="E207">
         <v>2.2032430784624299</v>
@@ -5811,13 +5811,13 @@
         <v>45913</v>
       </c>
       <c r="B208">
-        <v>2.0877735791338399</v>
+        <v>2.0878834735761398</v>
       </c>
       <c r="C208">
-        <v>44.9050876181742</v>
+        <v>44.917645470576403</v>
       </c>
       <c r="D208">
-        <v>4.4427462511123599</v>
+        <v>4.4417827444443096</v>
       </c>
       <c r="E208">
         <v>1.89504951238913</v>
@@ -5831,13 +5831,13 @@
         <v>45948</v>
       </c>
       <c r="B209">
-        <v>2.0994893776282102</v>
+        <v>2.0996550316080298</v>
       </c>
       <c r="C209">
-        <v>44.967914837983997</v>
+        <v>44.991378953943901</v>
       </c>
       <c r="D209">
-        <v>4.4606015832328598</v>
+        <v>4.4587150756813401</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
@@ -5845,13 +5845,13 @@
         <v>45976</v>
       </c>
       <c r="B210">
-        <v>2.0987120055698201</v>
+        <v>2.0991558556741099</v>
       </c>
       <c r="C210">
-        <v>44.951131386787999</v>
+        <v>44.962141949980001</v>
       </c>
       <c r="D210">
-        <v>4.4606142215357698</v>
+        <v>4.4604716689770303</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -5859,13 +5859,13 @@
         <v>46004</v>
       </c>
       <c r="B211">
-        <v>2.0941848560733698</v>
+        <v>2.0953250801779499</v>
       </c>
       <c r="C211">
-        <v>45.197235871461601</v>
+        <v>45.204885985112298</v>
       </c>
       <c r="D211">
-        <v>4.4282553238119302</v>
+        <v>4.4298429816427003</v>
       </c>
       <c r="E211">
         <v>2.0347166386895301</v>
@@ -5879,13 +5879,13 @@
         <v>46039</v>
       </c>
       <c r="B212">
-        <v>2.0720171581120099</v>
+        <v>2.07752877392713</v>
       </c>
       <c r="C212">
-        <v>45.2589617809098</v>
+        <v>45.098633362576699</v>
       </c>
       <c r="D212">
-        <v>4.3777187891707596</v>
+        <v>4.4037680893070998</v>
       </c>
     </row>
   </sheetData>
@@ -5902,7 +5902,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5911,7 +5911,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
+      <c r="A1" s="20"/>
       <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
@@ -5933,60 +5933,60 @@
       <c r="N1" s="37"/>
       <c r="O1" s="37"/>
       <c r="P1" s="38"/>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="22" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="23" t="s">
         <v>126</v>
       </c>
     </row>
@@ -6000,32 +6000,32 @@
       <c r="C3">
         <v>4.2300000000000004</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="21">
         <v>4.32</v>
       </c>
       <c r="E3">
         <v>4.41</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="18">
         <v>4.46</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="10">
         <v>4.2</v>
       </c>
       <c r="H3" s="1">
         <v>4.25</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="21">
         <v>4.34</v>
       </c>
       <c r="J3" s="1">
         <v>4.43</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="19">
         <v>4.4800000000000004</v>
       </c>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18">
         <v>4.4400000000000004</v>
       </c>
       <c r="S3" s="1"/>
@@ -6040,28 +6040,28 @@
       <c r="C4">
         <v>4.16</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="21">
         <v>4.3499999999999996</v>
       </c>
       <c r="E4">
         <v>4.53</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="19">
         <v>4.62</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="11">
         <v>4.08</v>
       </c>
       <c r="H4" s="1">
         <v>4.18</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="21">
         <v>4.3600000000000003</v>
       </c>
       <c r="J4" s="1">
         <v>4.54</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="19">
         <v>4.6399999999999997</v>
       </c>
       <c r="L4" s="1">
@@ -6076,10 +6076,10 @@
       <c r="O4" s="1">
         <v>4.55</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="19">
         <v>4.59</v>
       </c>
-      <c r="R4" s="20"/>
+      <c r="R4" s="15"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -6092,39 +6092,39 @@
       <c r="C5">
         <v>4.26</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="21">
         <v>4.4400000000000004</v>
       </c>
       <c r="E5">
         <v>4.62</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="19">
         <v>4.72</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="11">
         <v>4.16</v>
       </c>
       <c r="H5" s="1">
         <v>4.26</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="21">
         <v>4.4400000000000004</v>
       </c>
       <c r="J5" s="1">
         <v>4.62</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="19">
         <v>4.72</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="9"/>
+      <c r="P5" s="19"/>
       <c r="Q5">
         <v>4.54</v>
       </c>
-      <c r="R5" s="20"/>
+      <c r="R5" s="15"/>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -6137,13 +6137,13 @@
       <c r="C6">
         <v>4.46</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="21">
         <v>4.5599999999999996</v>
       </c>
       <c r="E6">
         <v>4.6399999999999997</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="19">
         <v>4.6900000000000004</v>
       </c>
       <c r="G6">
@@ -6152,17 +6152,17 @@
       <c r="H6">
         <v>4.47</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="21">
         <v>4.5599999999999996</v>
       </c>
       <c r="J6">
         <v>4.6500000000000004</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="12">
         <v>4.7</v>
       </c>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="18">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="13">
         <v>4.38</v>
       </c>
       <c r="S6" s="1"/>
@@ -6177,18 +6177,32 @@
       <c r="C7">
         <v>4.26</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="21">
         <v>4.3499999999999996</v>
       </c>
       <c r="E7">
         <v>4.4400000000000004</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="19">
         <v>4.49</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="K7" s="43"/>
-      <c r="P7" s="43"/>
+      <c r="G7">
+        <v>4.22</v>
+      </c>
+      <c r="H7">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="I7" s="21">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="J7">
+        <v>4.45</v>
+      </c>
+      <c r="K7" s="19">
+        <v>4.5</v>
+      </c>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="42"/>
       <c r="S7" s="1"/>
     </row>
   </sheetData>
@@ -6204,13 +6218,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6219,13 +6233,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="37" t="s">
         <v>53</v>
       </c>
       <c r="D1" s="38"/>
-      <c r="E1" s="11"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -6288,7 +6302,7 @@
       <c r="C5">
         <v>0.01</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="19">
         <v>0.01</v>
       </c>
       <c r="E5">
@@ -6308,7 +6322,7 @@
       <c r="C6">
         <v>0.02</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="19">
         <v>0.01</v>
       </c>
       <c r="E6">
@@ -6368,7 +6382,7 @@
       <c r="C9">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="19">
         <v>-2E-3</v>
       </c>
       <c r="E9" s="24">
@@ -6385,7 +6399,7 @@
       <c r="C10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="19">
         <v>-4.0000000000000001E-3</v>
       </c>
       <c r="E10" s="24">
@@ -6399,14 +6413,31 @@
       <c r="B11" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="24">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="12">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="E11" s="44">
-        <v>4.3544999999999998</v>
+      <c r="E11" s="24">
+        <v>4.3540000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>46039</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="44">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D12" s="45">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="E12" s="44">
+        <v>4.3630000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -6422,11 +6453,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6470,102 +6501,102 @@
       <c r="AC1" s="41"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="22" t="str">
+      <c r="K2" s="17" t="str">
         <f>"-0.4 to -0.2 pp"</f>
         <v>-0.4 to -0.2 pp</v>
       </c>
-      <c r="L2" s="22" t="str">
+      <c r="L2" s="17" t="str">
         <f>"-0.1 to +0.1 pp"</f>
         <v>-0.1 to +0.1 pp</v>
       </c>
-      <c r="M2" s="22" t="str">
+      <c r="M2" s="17" t="str">
         <f>"+0.2 to +0.4 pp"</f>
         <v>+0.2 to +0.4 pp</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="16" t="s">
         <v>60</v>
       </c>
       <c r="O2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="22" t="str">
+      <c r="P2" s="17" t="str">
         <f>"-0.6 pp"</f>
         <v>-0.6 pp</v>
       </c>
-      <c r="Q2" s="22" t="str">
+      <c r="Q2" s="17" t="str">
         <f>"-0.5 pp"</f>
         <v>-0.5 pp</v>
       </c>
-      <c r="R2" s="22" t="str">
+      <c r="R2" s="17" t="str">
         <f>"-0.4 pp"</f>
         <v>-0.4 pp</v>
       </c>
-      <c r="S2" s="22" t="str">
+      <c r="S2" s="17" t="str">
         <f>"-0.3 pp"</f>
         <v>-0.3 pp</v>
       </c>
-      <c r="T2" s="22" t="str">
+      <c r="T2" s="17" t="str">
         <f>"-0.2 pp"</f>
         <v>-0.2 pp</v>
       </c>
-      <c r="U2" s="22" t="str">
+      <c r="U2" s="17" t="str">
         <f>"-0.1 pp"</f>
         <v>-0.1 pp</v>
       </c>
       <c r="V2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="22" t="str">
+      <c r="W2" s="17" t="str">
         <f>"0.1 pp"</f>
         <v>0.1 pp</v>
       </c>
-      <c r="X2" s="22" t="str">
+      <c r="X2" s="17" t="str">
         <f>"0.2 pp"</f>
         <v>0.2 pp</v>
       </c>
-      <c r="Y2" s="22" t="str">
+      <c r="Y2" s="17" t="str">
         <f>"0.3 pp"</f>
         <v>0.3 pp</v>
       </c>
-      <c r="Z2" s="22" t="str">
+      <c r="Z2" s="17" t="str">
         <f>"0.4 pp"</f>
         <v>0.4 pp</v>
       </c>
-      <c r="AA2" s="22" t="str">
+      <c r="AA2" s="17" t="str">
         <f>"0.5 pp"</f>
         <v>0.5 pp</v>
       </c>
-      <c r="AB2" s="22" t="str">
+      <c r="AB2" s="17" t="str">
         <f>"0.6 pp"</f>
         <v>0.6 pp</v>
       </c>
@@ -6598,15 +6629,15 @@
       <c r="H3">
         <v>11</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="19">
         <v>5.9</v>
       </c>
-      <c r="J3" s="16"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="16"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="11"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -6620,7 +6651,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="9"/>
+      <c r="AC3" s="19"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -6647,15 +6678,15 @@
       <c r="H4">
         <v>12.8</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="19">
         <v>7.5</v>
       </c>
-      <c r="J4" s="16"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="16"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="11"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -6669,7 +6700,7 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
-      <c r="AC4" s="9"/>
+      <c r="AC4" s="19"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
@@ -6678,7 +6709,7 @@
       <c r="B5" t="s">
         <v>129</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="19"/>
       <c r="J5" s="32">
         <v>4.7</v>
       </c>
@@ -6708,7 +6739,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="9"/>
+      <c r="AC5" s="19"/>
       <c r="AD5" s="4" t="s">
         <v>58</v>
       </c>
@@ -6720,8 +6751,8 @@
       <c r="B6" t="s">
         <v>130</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="16">
+      <c r="I6" s="19"/>
+      <c r="J6" s="11">
         <v>4.5</v>
       </c>
       <c r="K6" s="1">
@@ -6733,10 +6764,10 @@
       <c r="M6" s="1">
         <v>27.7</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="19">
         <v>8.9</v>
       </c>
-      <c r="AC6" s="9"/>
+      <c r="AC6" s="19"/>
       <c r="AD6" s="4" t="s">
         <v>58</v>
       </c>
@@ -6748,9 +6779,9 @@
       <c r="B7" t="s">
         <v>129</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="16">
+      <c r="I7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="11">
         <v>2.7</v>
       </c>
       <c r="P7" s="1">
@@ -6792,7 +6823,7 @@
       <c r="AB7" s="1">
         <v>1.4</v>
       </c>
-      <c r="AC7" s="9">
+      <c r="AC7" s="19">
         <v>3.1</v>
       </c>
       <c r="AD7" s="4" t="s">
@@ -6806,9 +6837,9 @@
       <c r="B8" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="I8" s="9"/>
-      <c r="N8" s="9"/>
+      <c r="C8" s="11"/>
+      <c r="I8" s="19"/>
+      <c r="N8" s="19"/>
       <c r="O8">
         <v>2.7</v>
       </c>
@@ -6851,7 +6882,7 @@
       <c r="AB8">
         <v>1.4</v>
       </c>
-      <c r="AC8" s="9">
+      <c r="AC8" s="19">
         <v>3.1</v>
       </c>
       <c r="AD8" s="4"/>
@@ -6881,11 +6912,11 @@
       <c r="H9">
         <v>5.5</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="19">
         <v>3.2</v>
       </c>
-      <c r="N9" s="9"/>
-      <c r="AC9" s="9"/>
+      <c r="N9" s="19"/>
+      <c r="AC9" s="19"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
@@ -6912,11 +6943,11 @@
       <c r="H10">
         <v>6.1</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="19">
         <v>3.4</v>
       </c>
-      <c r="N10" s="9"/>
-      <c r="AC10" s="9"/>
+      <c r="N10" s="19"/>
+      <c r="AC10" s="19"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
@@ -6946,9 +6977,40 @@
       <c r="I11">
         <v>3.3</v>
       </c>
-      <c r="J11" s="42"/>
-      <c r="N11" s="43"/>
-      <c r="AC11" s="43"/>
+      <c r="J11" s="11"/>
+      <c r="N11" s="19"/>
+      <c r="AC11" s="19"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>46039</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12">
+        <v>7.5</v>
+      </c>
+      <c r="D12">
+        <v>13.3</v>
+      </c>
+      <c r="E12">
+        <v>26.1</v>
+      </c>
+      <c r="F12">
+        <v>27.7</v>
+      </c>
+      <c r="G12">
+        <v>15.7</v>
+      </c>
+      <c r="H12">
+        <v>6.2</v>
+      </c>
+      <c r="I12" s="43">
+        <v>3.5</v>
+      </c>
+      <c r="N12" s="43"/>
+      <c r="AC12" s="43"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="L15" s="1"/>

</xml_diff>